<commit_message>
commit to muskan branch
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="72">
   <si>
     <t>TestData</t>
   </si>
@@ -160,7 +160,7 @@
     <t>Upma@007</t>
   </si>
   <si>
-    <t>Automation-testing18</t>
+    <t>Automation-testing19</t>
   </si>
   <si>
     <t>Testdata10</t>
@@ -205,10 +205,13 @@
     <t>NA</t>
   </si>
   <si>
+    <t>Ram Roy</t>
+  </si>
+  <si>
+    <t>Testdata28</t>
+  </si>
+  <si>
     <t>Rahul Roy</t>
-  </si>
-  <si>
-    <t>Testdata28</t>
   </si>
   <si>
     <t>Testdata26</t>
@@ -234,10 +237,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="178" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="25">
     <font>
@@ -288,8 +291,84 @@
       <charset val="134"/>
     </font>
     <font>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF006100"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -304,6 +383,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
@@ -311,7 +398,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -327,91 +414,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -439,31 +442,145 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -475,145 +592,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -663,7 +666,37 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
       </bottom>
       <diagonal/>
     </border>
@@ -679,6 +712,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -709,45 +751,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -759,7 +762,10 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -771,136 +777,133 @@
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="16" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1176,8 +1179,8 @@
   <sheetPr/>
   <dimension ref="A1:T24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+    <sheetView tabSelected="1" topLeftCell="L4" workbookViewId="0">
+      <selection activeCell="O13" sqref="O13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.87272727272727" defaultRowHeight="13.5" customHeight="1"/>
@@ -2060,12 +2063,12 @@
         <v>62</v>
       </c>
       <c r="P22" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
     </row>
     <row r="23" customHeight="1" spans="1:15">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>17</v>
@@ -2095,24 +2098,24 @@
         <v>25</v>
       </c>
       <c r="K23" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="L23" t="s">
         <v>31</v>
       </c>
       <c r="M23" s="4" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N23" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O23" s="6" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
     <row r="24" customHeight="1" spans="1:11">
       <c r="A24" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>17</v>
@@ -2139,7 +2142,7 @@
         <v>24</v>
       </c>
       <c r="K24" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Commit Mobile test cases and necessary framework changes
Commit Mobile test cases and necessary framework changes
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6830" activeTab="2"/>
+    <workbookView windowWidth="27945" windowHeight="12210" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ACS" sheetId="8" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="882" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="239">
   <si>
     <t>TestData</t>
   </si>
@@ -507,6 +507,99 @@
     <t>Zoye</t>
   </si>
   <si>
+    <t>Testdata23</t>
+  </si>
+  <si>
+    <t>Tx-Testing</t>
+  </si>
+  <si>
+    <t>rahul1234@yopmail.com</t>
+  </si>
+  <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>10/JAN/2001</t>
+  </si>
+  <si>
+    <t>Ask about activities that they do with others,Ask demographic questions</t>
+  </si>
+  <si>
+    <t>Testdata24</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tx-Testing32</t>
+    </r>
+  </si>
+  <si>
+    <t>Tx-Testing4850</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Preet</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Kour</t>
+    </r>
+  </si>
+  <si>
+    <t>preet98@yopmail.com</t>
+  </si>
+  <si>
+    <t>160101</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>stroke</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Female</t>
+    </r>
+  </si>
+  <si>
     <t>TX_14</t>
   </si>
   <si>
@@ -654,9 +747,6 @@
     <t>John</t>
   </si>
   <si>
-    <t>160101</t>
-  </si>
-  <si>
     <t>14/SEP/2008</t>
   </si>
   <si>
@@ -672,27 +762,37 @@
     <t>Rahul</t>
   </si>
   <si>
-    <t>123456</t>
-  </si>
-  <si>
     <t>Rahul98@yopmail.com</t>
   </si>
   <si>
     <t>10</t>
+  </si>
+  <si>
+    <t>Testdata33</t>
+  </si>
+  <si>
+    <t>Sharma</t>
+  </si>
+  <si>
+    <t>Tx-Testing2201</t>
+  </si>
+  <si>
+    <t>Tx-Testing2422</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9">
-  <numFmts count="5">
+  <numFmts count="6">
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ &quot;₹&quot;* #,##0.00_ ;_ &quot;₹&quot;* \-#,##0.00_ ;_ &quot;₹&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
+    <numFmt numFmtId="181" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="28">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -705,35 +805,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <color rgb="FF454A4A"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1278,134 +1349,134 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1414,10 +1485,9 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1427,21 +1497,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1707,27 +1777,27 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90909090909091" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.5454545454545" customWidth="1"/>
-    <col min="2" max="2" width="49.4545454545455" customWidth="1"/>
-    <col min="3" max="3" width="26" customWidth="1"/>
-    <col min="4" max="4" width="11.0909090909091" customWidth="1"/>
-    <col min="5" max="5" width="19" customWidth="1"/>
-    <col min="6" max="6" width="33.1818181818182" customWidth="1"/>
-    <col min="7" max="7" width="24.6363636363636" customWidth="1"/>
-    <col min="8" max="8" width="19" customWidth="1"/>
-    <col min="9" max="9" width="19.7272727272727" customWidth="1"/>
-    <col min="10" max="10" width="64.2727272727273" customWidth="1"/>
-    <col min="11" max="11" width="28.1818181818182" customWidth="1"/>
-    <col min="12" max="12" width="102.181818181818" customWidth="1"/>
-    <col min="15" max="15" width="19.9090909090909" customWidth="1"/>
-    <col min="16" max="16" width="26.6363636363636" customWidth="1"/>
-    <col min="17" max="17" width="30.5454545454545" customWidth="1"/>
-    <col min="18" max="18" width="25.8181818181818" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="13.5428571428571" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="49.4571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="11.0952380952381" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="33.1809523809524" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.6380952380952" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="19.0" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="19.7238095238095" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="64.2761904761905" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="28.1809523809524" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="102.180952380952" collapsed="true"/>
+    <col min="15" max="15" customWidth="true" width="19.9047619047619" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="26.6380952380952" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="30.5428571428571" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="25.8190476190476" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.5" spans="1:18">
+    <row r="1" ht="15" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1783,7 +1853,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="14.5" spans="1:11">
+    <row r="2" ht="15" spans="1:11">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -1818,7 +1888,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" ht="14.5" spans="1:12">
+    <row r="3" ht="15" spans="1:12">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -1852,11 +1922,11 @@
       <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="22" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" ht="14.5" spans="1:12">
+    <row r="4" ht="15" spans="1:12">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -1894,7 +1964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" ht="14.5" spans="1:12">
+    <row r="5" ht="15" spans="1:12">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -1928,7 +1998,7 @@
       <c r="K5" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="25" t="s">
+      <c r="L5" s="22" t="s">
         <v>36</v>
       </c>
     </row>
@@ -1966,11 +2036,11 @@
       <c r="K6" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="25" t="s">
+      <c r="L6" s="22" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="T6" s="25"/>
+      <c r="T6" s="22"/>
     </row>
     <row r="7" customHeight="1" spans="1:12">
       <c r="A7" t="s">
@@ -2038,7 +2108,7 @@
       <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K8" t="s">
@@ -2073,13 +2143,13 @@
       <c r="I9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K9" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="25" t="s">
+      <c r="L9" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2111,7 +2181,7 @@
       <c r="I10" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K10" t="s">
@@ -2146,7 +2216,7 @@
       <c r="I11" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K11" t="s">
@@ -2184,13 +2254,13 @@
       <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K12" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="25" t="s">
+      <c r="L12" s="22" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2222,13 +2292,13 @@
       <c r="I13" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K13" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2260,7 +2330,7 @@
       <c r="I14" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K14" t="s">
@@ -2339,7 +2409,7 @@
       <c r="K16" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="25" t="s">
+      <c r="L16" s="22" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2415,7 +2485,7 @@
       <c r="K18" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="25" t="s">
+      <c r="L18" s="22" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2453,7 +2523,7 @@
       <c r="K19" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="25" t="s">
+      <c r="L19" s="22" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2523,7 +2593,7 @@
       <c r="I21" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K21" t="s">
@@ -2541,7 +2611,7 @@
       <c r="O21" t="s">
         <v>63</v>
       </c>
-      <c r="P21" s="26" t="s">
+      <c r="P21" s="23" t="s">
         <v>64</v>
       </c>
       <c r="Q21" s="3" t="s">
@@ -2579,7 +2649,7 @@
       <c r="I22" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="23" t="s">
         <v>45</v>
       </c>
       <c r="K22" t="s">
@@ -2788,19 +2858,19 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="53.4545454545455" customWidth="1"/>
-    <col min="3" max="3" width="41.0909090909091" customWidth="1"/>
-    <col min="4" max="4" width="19.8181818181818" customWidth="1"/>
-    <col min="5" max="6" width="24.5454545454545" customWidth="1"/>
-    <col min="7" max="7" width="30.8181818181818" customWidth="1"/>
-    <col min="8" max="8" width="14.2727272727273" customWidth="1"/>
-    <col min="9" max="9" width="35.4545454545455" customWidth="1"/>
-    <col min="10" max="10" width="41.4545454545455" customWidth="1"/>
-    <col min="11" max="11" width="27.8181818181818" customWidth="1"/>
-    <col min="14" max="14" width="16.4545454545455" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="53.4571428571429" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="41.0952380952381" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.8190476190476" collapsed="true"/>
+    <col min="5" max="6" customWidth="true" width="24.5428571428571" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.8190476190476" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="14.2761904761905" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="35.4571428571429" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="41.4571428571429" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="27.8190476190476" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="16.4571428571429" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2901,13 +2971,13 @@
       <c r="H3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="23" t="s">
+      <c r="I3" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="23" t="s">
+      <c r="K3" s="20" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2942,7 +3012,7 @@
       <c r="J4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="22" t="s">
+      <c r="K4" s="19" t="s">
         <v>66</v>
       </c>
     </row>
@@ -2956,7 +3026,7 @@
       <c r="C5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="19" t="s">
         <v>66</v>
       </c>
       <c r="E5" t="s">
@@ -3076,7 +3146,7 @@
       <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="27" t="s">
+      <c r="I8" s="24" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3252,39 +3322,39 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:Y30"/>
+  <dimension ref="A1:AB33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B34" sqref="B34"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="AA18" sqref="AA18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.4545454545455" customWidth="1"/>
-    <col min="2" max="2" width="52.8181818181818" customWidth="1"/>
-    <col min="3" max="3" width="38.9090909090909" customWidth="1"/>
-    <col min="4" max="4" width="18.2727272727273" customWidth="1"/>
-    <col min="5" max="5" width="23.4545454545455" customWidth="1"/>
-    <col min="6" max="6" width="17.6363636363636" customWidth="1"/>
-    <col min="7" max="7" width="41.1818181818182" customWidth="1"/>
-    <col min="8" max="8" width="22.3636363636364" customWidth="1"/>
-    <col min="9" max="9" width="24.8181818181818" customWidth="1"/>
-    <col min="10" max="10" width="17" customWidth="1"/>
-    <col min="11" max="11" width="15.3636363636364" customWidth="1"/>
-    <col min="12" max="12" width="26.6363636363636" customWidth="1"/>
-    <col min="13" max="13" width="15.3636363636364" customWidth="1"/>
-    <col min="14" max="14" width="13.7272727272727" customWidth="1"/>
-    <col min="16" max="16" width="17.4545454545455" customWidth="1"/>
-    <col min="18" max="18" width="26.3636363636364" customWidth="1"/>
-    <col min="19" max="19" width="23.5454545454545" customWidth="1"/>
-    <col min="20" max="20" width="18.7272727272727" customWidth="1"/>
-    <col min="21" max="21" width="16.4545454545455" customWidth="1"/>
-    <col min="22" max="22" width="13.0909090909091" customWidth="1"/>
-    <col min="23" max="23" width="13.5454545454545" customWidth="1"/>
-    <col min="24" max="24" width="13.9090909090909" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="16.4571428571429" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="52.8190476190476" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="38.9047619047619" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="18.2761904761905" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.4571428571429" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="17.6380952380952" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="41.1809523809524" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="22.3619047619048" collapsed="true"/>
+    <col min="9" max="9" customWidth="true" width="24.8190476190476" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="15.3619047619048" collapsed="true"/>
+    <col min="12" max="12" customWidth="true" width="26.6380952380952" collapsed="true"/>
+    <col min="13" max="13" customWidth="true" width="15.3619047619048" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" width="13.7238095238095" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="17.4571428571429" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="26.3619047619048" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" width="23.5428571428571" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="18.7238095238095" collapsed="true"/>
+    <col min="21" max="21" customWidth="true" width="16.4571428571429" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" width="13.0952380952381" collapsed="true"/>
+    <col min="23" max="23" customWidth="true" width="13.5428571428571" collapsed="true"/>
+    <col min="24" max="24" customWidth="true" width="13.9047619047619" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25">
+    <row r="1" spans="1:28">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3359,6 +3429,15 @@
       </c>
       <c r="Y1" t="s">
         <v>120</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>16</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:9">
@@ -3485,16 +3564,16 @@
       <c r="L5" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="M5" s="12" t="s">
+      <c r="M5" s="9" t="s">
         <v>128</v>
       </c>
       <c r="N5" t="s">
         <v>129</v>
       </c>
-      <c r="O5" s="12" t="s">
+      <c r="O5" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="P5" s="13" t="s">
+      <c r="P5" s="10" t="s">
         <v>131</v>
       </c>
       <c r="Q5" t="s">
@@ -3538,16 +3617,16 @@
       <c r="L6" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="12" t="s">
+      <c r="M6" s="9" t="s">
         <v>128</v>
       </c>
       <c r="N6" t="s">
         <v>129</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="P6" s="13" t="s">
+      <c r="P6" s="10" t="s">
         <v>131</v>
       </c>
       <c r="Q6" t="s">
@@ -3591,16 +3670,16 @@
       <c r="L7" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="M7" s="12" t="s">
+      <c r="M7" s="9" t="s">
         <v>128</v>
       </c>
       <c r="N7" t="s">
         <v>129</v>
       </c>
-      <c r="O7" s="12" t="s">
+      <c r="O7" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="P7" s="13" t="s">
+      <c r="P7" s="10" t="s">
         <v>131</v>
       </c>
       <c r="Q7" t="s">
@@ -3644,8 +3723,8 @@
       <c r="L8" t="s">
         <v>129</v>
       </c>
-      <c r="M8" s="12"/>
-      <c r="N8" s="13" t="s">
+      <c r="M8" s="9"/>
+      <c r="N8" s="10" t="s">
         <v>131</v>
       </c>
       <c r="O8" t="s">
@@ -3663,7 +3742,7 @@
       <c r="S8" t="s">
         <v>124</v>
       </c>
-      <c r="T8" s="19" t="s">
+      <c r="T8" s="16" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3728,16 +3807,16 @@
       <c r="L10" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="M10" s="12" t="s">
+      <c r="M10" s="9" t="s">
         <v>128</v>
       </c>
       <c r="N10" t="s">
         <v>129</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="9" t="s">
         <v>130</v>
       </c>
-      <c r="P10" s="13" t="s">
+      <c r="P10" s="10" t="s">
         <v>131</v>
       </c>
       <c r="Q10" t="s">
@@ -3790,7 +3869,7 @@
       <c r="O11">
         <v>1122</v>
       </c>
-      <c r="P11" s="14">
+      <c r="P11" s="11">
         <v>29749</v>
       </c>
       <c r="Q11" t="s">
@@ -3945,7 +4024,7 @@
       <c r="L15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="M15" s="15" t="s">
+      <c r="M15" s="12" t="s">
         <v>155</v>
       </c>
       <c r="N15" s="7" t="s">
@@ -3954,7 +4033,7 @@
       <c r="O15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="P15" s="16" t="s">
+      <c r="P15" s="13" t="s">
         <v>156</v>
       </c>
       <c r="Q15" s="7" t="s">
@@ -4034,9 +4113,9 @@
         <v>162</v>
       </c>
     </row>
-    <row r="18" spans="1:10">
-      <c r="A18" s="7" t="s">
-        <v>75</v>
+    <row r="18" spans="1:28">
+      <c r="A18" t="s">
+        <v>163</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>19</v>
@@ -4047,11 +4126,11 @@
       <c r="D18" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E18" s="6" t="s">
-        <v>163</v>
-      </c>
-      <c r="F18" s="7" t="s">
-        <v>63</v>
+      <c r="E18" t="s">
+        <v>164</v>
+      </c>
+      <c r="F18" t="s">
+        <v>133</v>
       </c>
       <c r="G18" t="s">
         <v>63</v>
@@ -4062,28 +4141,82 @@
       <c r="I18" t="s">
         <v>63</v>
       </c>
-      <c r="J18" s="6" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10">
-      <c r="A19" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C19" s="3" t="s">
+      <c r="J18" t="s">
+        <v>150</v>
+      </c>
+      <c r="K18" t="s">
+        <v>151</v>
+      </c>
+      <c r="L18" t="s">
+        <v>165</v>
+      </c>
+      <c r="M18" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="N18" t="s">
+        <v>129</v>
+      </c>
+      <c r="O18" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="P18" s="15" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q18" t="s">
+        <v>132</v>
+      </c>
+      <c r="R18" t="s">
+        <v>63</v>
+      </c>
+      <c r="S18" t="s">
+        <v>63</v>
+      </c>
+      <c r="T18" t="s">
+        <v>63</v>
+      </c>
+      <c r="U18" t="s">
+        <v>63</v>
+      </c>
+      <c r="V18" t="s">
+        <v>63</v>
+      </c>
+      <c r="W18" t="s">
+        <v>63</v>
+      </c>
+      <c r="X18" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>169</v>
+      </c>
+      <c r="AA18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="AB18" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="E19" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="F19" s="7" t="s">
-        <v>63</v>
+    </row>
+    <row r="19" spans="1:28">
+      <c r="A19" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="C19" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="E19" s="8" t="s">
+        <v>171</v>
+      </c>
+      <c r="F19" t="s">
+        <v>238</v>
       </c>
       <c r="G19" t="s">
         <v>63</v>
@@ -4094,13 +4227,67 @@
       <c r="I19" t="s">
         <v>63</v>
       </c>
-      <c r="J19" t="s">
-        <v>164</v>
+      <c r="J19" s="8" t="s">
+        <v>173</v>
+      </c>
+      <c r="K19" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="L19" s="8" t="s">
+        <v>175</v>
+      </c>
+      <c r="M19" s="14" t="s">
+        <v>176</v>
+      </c>
+      <c r="N19" s="8" t="s">
+        <v>177</v>
+      </c>
+      <c r="O19" s="14" t="s">
+        <v>167</v>
+      </c>
+      <c r="P19" s="15" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q19" s="8" t="s">
+        <v>178</v>
+      </c>
+      <c r="R19" t="s">
+        <v>63</v>
+      </c>
+      <c r="S19" t="s">
+        <v>63</v>
+      </c>
+      <c r="T19" t="s">
+        <v>63</v>
+      </c>
+      <c r="U19" t="s">
+        <v>63</v>
+      </c>
+      <c r="V19" t="s">
+        <v>63</v>
+      </c>
+      <c r="W19" t="s">
+        <v>63</v>
+      </c>
+      <c r="X19" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB19" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="20" spans="1:10">
       <c r="A20" s="7" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>19</v>
@@ -4112,7 +4299,7 @@
         <v>21</v>
       </c>
       <c r="E20" s="6" t="s">
-        <v>166</v>
+        <v>179</v>
       </c>
       <c r="F20" s="7" t="s">
         <v>63</v>
@@ -4126,13 +4313,13 @@
       <c r="I20" t="s">
         <v>63</v>
       </c>
-      <c r="J20" t="s">
-        <v>164</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7">
+      <c r="J20" s="6" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10">
       <c r="A21" s="7" t="s">
-        <v>167</v>
+        <v>70</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>19</v>
@@ -4144,82 +4331,59 @@
         <v>21</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>168</v>
-      </c>
-      <c r="F21" t="s">
-        <v>169</v>
-      </c>
-      <c r="G21" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="22" spans="1:25">
-      <c r="A22" s="8" t="s">
-        <v>170</v>
-      </c>
-      <c r="B22" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C22" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="F21" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G21" t="s">
+        <v>63</v>
+      </c>
+      <c r="H21" t="s">
+        <v>63</v>
+      </c>
+      <c r="I21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J21" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10">
+      <c r="A22" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C22" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="10" t="s">
+      <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E22" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="F22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="H22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="I22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J22" s="11" t="s">
-        <v>164</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M22" s="17">
-        <v>500018</v>
-      </c>
-      <c r="N22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P22" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q22" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="R22" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="S22" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="U22" s="13"/>
-      <c r="V22" s="13"/>
-      <c r="W22" s="13"/>
-      <c r="X22" s="13"/>
-      <c r="Y22" s="13"/>
-    </row>
-    <row r="23" spans="1:19">
+      <c r="E22" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="F22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G22" t="s">
+        <v>63</v>
+      </c>
+      <c r="H22" t="s">
+        <v>63</v>
+      </c>
+      <c r="I22" t="s">
+        <v>63</v>
+      </c>
+      <c r="J22" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="7" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>19</v>
@@ -4231,42 +4395,18 @@
         <v>21</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>175</v>
-      </c>
-      <c r="J23" s="6" t="s">
-        <v>176</v>
-      </c>
-      <c r="K23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M23" s="15" t="s">
-        <v>155</v>
-      </c>
-      <c r="N23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P23" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q23" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R23" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="S23" s="4" t="s">
-        <v>177</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10">
+        <v>184</v>
+      </c>
+      <c r="F23" t="s">
+        <v>185</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25">
       <c r="A24" s="7" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>19</v>
@@ -4278,183 +4418,140 @@
         <v>21</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>180</v>
+        <v>187</v>
+      </c>
+      <c r="F24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I24" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="J24" s="6" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="25" spans="1:25">
-      <c r="A25" s="8" t="s">
-        <v>181</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C25" s="9" t="s">
+      <c r="K24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="12">
+        <v>500018</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S24" s="6" t="s">
+        <v>189</v>
+      </c>
+      <c r="U24" s="10"/>
+      <c r="V24" s="10"/>
+      <c r="W24" s="10"/>
+      <c r="X24" s="10"/>
+      <c r="Y24" s="10"/>
+    </row>
+    <row r="25" spans="1:19">
+      <c r="A25" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C25" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D25" s="10" t="s">
+      <c r="D25" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E25" s="11" t="s">
-        <v>182</v>
-      </c>
-      <c r="F25" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" t="s">
-        <v>63</v>
-      </c>
-      <c r="H25" t="s">
-        <v>63</v>
-      </c>
-      <c r="I25" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="11" t="s">
-        <v>183</v>
-      </c>
-      <c r="K25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="R25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="S25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="T25" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="U25" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="V25" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="W25" s="13" t="s">
-        <v>185</v>
-      </c>
-      <c r="X25" s="13" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y25" s="13" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="26" spans="1:25">
-      <c r="A26" s="8" t="s">
+      <c r="E25" s="6" t="s">
+        <v>191</v>
+      </c>
+      <c r="J25" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="K25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="N25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P25" s="13" t="s">
         <v>188</v>
       </c>
-      <c r="B26" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C26" s="9" t="s">
+      <c r="Q25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R25" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S25" s="4" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10">
+      <c r="A26" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C26" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D26" s="10" t="s">
+      <c r="D26" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>189</v>
-      </c>
-      <c r="F26" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" t="s">
-        <v>63</v>
-      </c>
-      <c r="H26" t="s">
-        <v>63</v>
-      </c>
-      <c r="I26" t="s">
-        <v>63</v>
-      </c>
-      <c r="J26" s="11" t="s">
-        <v>190</v>
-      </c>
-      <c r="K26" t="s">
-        <v>63</v>
-      </c>
-      <c r="L26" t="s">
-        <v>63</v>
-      </c>
-      <c r="M26" s="17" t="s">
-        <v>191</v>
-      </c>
-      <c r="N26" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O26" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P26" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q26" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="R26" t="s">
-        <v>157</v>
-      </c>
-      <c r="S26" s="20" t="s">
-        <v>192</v>
-      </c>
-      <c r="T26" t="s">
-        <v>63</v>
-      </c>
-      <c r="U26" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="V26" s="13" t="s">
-        <v>193</v>
-      </c>
-      <c r="W26" s="13" t="s">
-        <v>194</v>
-      </c>
-      <c r="X26" s="13" t="s">
+      <c r="E26" s="6" t="s">
         <v>195</v>
       </c>
-      <c r="Y26" s="13" t="s">
+      <c r="F26" s="6" t="s">
         <v>196</v>
       </c>
+      <c r="J26" s="6" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="27" spans="1:25">
-      <c r="A27" s="8" t="s">
+      <c r="A27" s="7" t="s">
         <v>197</v>
       </c>
-      <c r="B27" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C27" s="9" t="s">
+      <c r="B27" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C27" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="10" t="s">
+      <c r="D27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="6" t="s">
         <v>198</v>
       </c>
       <c r="F27" t="s">
@@ -4469,70 +4566,70 @@
       <c r="I27" t="s">
         <v>63</v>
       </c>
-      <c r="J27" s="11" t="s">
+      <c r="J27" s="6" t="s">
         <v>199</v>
       </c>
-      <c r="K27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="N27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="R27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="S27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="T27" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="U27" s="18" t="s">
-        <v>184</v>
-      </c>
-      <c r="V27" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="W27" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="X27" s="18" t="s">
+      <c r="K27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U27" s="10" t="s">
         <v>200</v>
       </c>
-      <c r="Y27" s="18" t="s">
-        <v>196</v>
+      <c r="V27" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="W27" s="10" t="s">
+        <v>201</v>
+      </c>
+      <c r="X27" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y27" s="10" t="s">
+        <v>203</v>
       </c>
     </row>
     <row r="28" spans="1:25">
-      <c r="A28" s="8" t="s">
-        <v>201</v>
-      </c>
-      <c r="B28" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C28" s="9" t="s">
+      <c r="A28" s="7" t="s">
+        <v>204</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C28" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D28" s="10" t="s">
+      <c r="D28" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E28" s="11" t="s">
-        <v>202</v>
+      <c r="E28" s="6" t="s">
+        <v>205</v>
       </c>
       <c r="F28" t="s">
         <v>63</v>
@@ -4546,207 +4643,438 @@
       <c r="I28" t="s">
         <v>63</v>
       </c>
-      <c r="J28" s="11" t="s">
-        <v>203</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L28" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M28" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="N28" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O28" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P28" s="18" t="s">
-        <v>172</v>
-      </c>
-      <c r="Q28" s="8" t="s">
+      <c r="J28" s="6" t="s">
+        <v>206</v>
+      </c>
+      <c r="K28" t="s">
+        <v>63</v>
+      </c>
+      <c r="L28" t="s">
+        <v>63</v>
+      </c>
+      <c r="M28" s="12" t="s">
+        <v>207</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P28" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q28" s="7" t="s">
         <v>63</v>
       </c>
       <c r="R28" t="s">
         <v>157</v>
       </c>
-      <c r="S28" s="11" t="s">
-        <v>205</v>
-      </c>
-      <c r="T28" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="U28" s="18" t="s">
-        <v>206</v>
-      </c>
-      <c r="V28" s="18" t="s">
-        <v>207</v>
-      </c>
-      <c r="W28" s="18" t="s">
+      <c r="S28" s="4" t="s">
         <v>208</v>
       </c>
-      <c r="X28" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="Y28" s="18" t="s">
+      <c r="T28" t="s">
+        <v>63</v>
+      </c>
+      <c r="U28" s="10" t="s">
         <v>200</v>
       </c>
+      <c r="V28" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="W28" s="10" t="s">
+        <v>210</v>
+      </c>
+      <c r="X28" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y28" s="10" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="29" spans="1:25">
-      <c r="A29" s="8" t="s">
+      <c r="A29" s="7" t="s">
+        <v>213</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="F29" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" s="6" t="s">
+        <v>215</v>
+      </c>
+      <c r="K29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T29" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U29" s="13" t="s">
+        <v>200</v>
+      </c>
+      <c r="V29" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="W29" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="X29" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y29" s="13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="30" spans="1:25">
+      <c r="A30" s="7" t="s">
+        <v>217</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>218</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" s="12" t="s">
+        <v>220</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P30" s="13" t="s">
+        <v>188</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R30" t="s">
+        <v>157</v>
+      </c>
+      <c r="S30" s="6" t="s">
+        <v>221</v>
+      </c>
+      <c r="T30" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U30" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="V30" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="W30" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="X30" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y30" s="13" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:25">
+      <c r="A31" s="7" t="s">
+        <v>225</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" s="6" t="s">
+        <v>226</v>
+      </c>
+      <c r="F31" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" t="s">
+        <v>63</v>
+      </c>
+      <c r="H31" t="s">
+        <v>63</v>
+      </c>
+      <c r="I31" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="6" t="s">
+        <v>227</v>
+      </c>
+      <c r="K31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="N31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P31" s="13" t="s">
+        <v>228</v>
+      </c>
+      <c r="Q31" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R31" t="s">
+        <v>157</v>
+      </c>
+      <c r="S31" s="6" t="s">
+        <v>229</v>
+      </c>
+      <c r="T31" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="U31" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="V31" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="W31" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="X31" s="13" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y31" s="13" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25">
+      <c r="A32" s="7" t="s">
+        <v>230</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C32" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" s="6" t="s">
+        <v>231</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G32" t="s">
+        <v>63</v>
+      </c>
+      <c r="H32" t="s">
+        <v>63</v>
+      </c>
+      <c r="I32" t="s">
+        <v>63</v>
+      </c>
+      <c r="J32" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="K32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M32" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="N32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P32" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R32" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S32" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="T32" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U32" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="V32" s="13" t="s">
         <v>209</v>
       </c>
-      <c r="B29" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C29" s="9" t="s">
+      <c r="W32" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="X32" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y32" s="13" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="33" spans="1:25">
+      <c r="A33" t="s">
+        <v>235</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C33" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D29" s="10" t="s">
+      <c r="D33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>210</v>
-      </c>
-      <c r="F29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="11" t="s">
-        <v>211</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M29" s="17" t="s">
+      <c r="E33" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G33" t="s">
+        <v>63</v>
+      </c>
+      <c r="H33" t="s">
+        <v>63</v>
+      </c>
+      <c r="I33" t="s">
+        <v>63</v>
+      </c>
+      <c r="J33" t="s">
+        <v>232</v>
+      </c>
+      <c r="K33" t="s">
+        <v>236</v>
+      </c>
+      <c r="L33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="N33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O33" s="9" t="s">
+        <v>167</v>
+      </c>
+      <c r="P33" s="13" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R33" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S33" s="17" t="s">
+        <v>233</v>
+      </c>
+      <c r="T33" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U33" s="10" t="s">
+        <v>200</v>
+      </c>
+      <c r="V33" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="W33" s="13" t="s">
+        <v>234</v>
+      </c>
+      <c r="X33" s="13" t="s">
+        <v>216</v>
+      </c>
+      <c r="Y33" s="13" t="s">
         <v>212</v>
-      </c>
-      <c r="N29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P29" s="18" t="s">
-        <v>213</v>
-      </c>
-      <c r="Q29" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="R29" t="s">
-        <v>157</v>
-      </c>
-      <c r="S29" s="11" t="s">
-        <v>214</v>
-      </c>
-      <c r="T29" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="U29" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="V29" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="W29" s="18" t="s">
-        <v>185</v>
-      </c>
-      <c r="X29" s="18" t="s">
-        <v>186</v>
-      </c>
-      <c r="Y29" s="18" t="s">
-        <v>187</v>
-      </c>
-    </row>
-    <row r="30" spans="1:25">
-      <c r="A30" s="8" t="s">
-        <v>215</v>
-      </c>
-      <c r="B30" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C30" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="E30" s="11" t="s">
-        <v>216</v>
-      </c>
-      <c r="F30" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" s="11" t="s">
-        <v>217</v>
-      </c>
-      <c r="K30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="L30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="M30" s="17" t="s">
-        <v>218</v>
-      </c>
-      <c r="N30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="O30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="P30" s="18" t="s">
-        <v>131</v>
-      </c>
-      <c r="Q30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="R30" s="8" t="s">
-        <v>157</v>
-      </c>
-      <c r="S30" s="21" t="s">
-        <v>219</v>
-      </c>
-      <c r="T30" s="8" t="s">
-        <v>63</v>
-      </c>
-      <c r="U30" s="13" t="s">
-        <v>184</v>
-      </c>
-      <c r="V30" s="18" t="s">
-        <v>193</v>
-      </c>
-      <c r="W30" s="18" t="s">
-        <v>220</v>
-      </c>
-      <c r="X30" s="18" t="s">
-        <v>200</v>
-      </c>
-      <c r="Y30" s="18" t="s">
-        <v>196</v>
       </c>
     </row>
   </sheetData>
@@ -4788,15 +5116,15 @@
     <hyperlink ref="B17" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D17" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C17" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="B18" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D18" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C18" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="B19" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D19" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C19" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B20" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D20" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C20" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B21" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D21" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C21" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B22" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D22" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C22" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="L10" r:id="rId8" display="rahul@gamil.com"/>
     <hyperlink ref="B8" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="C8" r:id="rId4" display="amandeep.kamboj@testingxperts.com"/>
@@ -4805,15 +5133,9 @@
     <hyperlink ref="C11" r:id="rId9" display="dhanya@yopmail.com"/>
     <hyperlink ref="L11" r:id="rId10" display="shardha@yopmail.com"/>
     <hyperlink ref="B12" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="B21" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D21" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C21" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B23" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D23" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C23" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="B24" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D24" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C24" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B25" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D25" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C25" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
@@ -4823,19 +5145,37 @@
     <hyperlink ref="B27" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D27" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C27" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="S26" r:id="rId11" display="ajay@yopmail.com"/>
     <hyperlink ref="B28" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D28" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C28" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B29" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D29" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C29" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="S28" r:id="rId11" display="ajay@yopmail.com"/>
     <hyperlink ref="B30" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D30" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C30" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="D30" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="B22" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="C22" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="D22" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="B31" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D31" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C31" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B32" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C32" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D32" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="B24" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C24" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D24" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="B33" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C33" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D33" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="D18" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C18" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B18" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="AB18" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="AA18" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B19" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C19" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D19" r:id="rId12" display="Sah@6057" tooltip="mailto:Sah@6057"/>
+    <hyperlink ref="L19" r:id="rId13" display="preet98@yopmail.com" tooltip="mailto:preet98@yopmail.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
comitting the mobile related test cases till 50
Committing all the mobile test cases till 50th
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="968" uniqueCount="239">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1262" uniqueCount="291">
   <si>
     <t>TestData</t>
   </si>
@@ -543,7 +543,7 @@
     </r>
   </si>
   <si>
-    <t>Tx-Testing4850</t>
+    <t>Tx-Testing2422</t>
   </si>
   <si>
     <r>
@@ -612,6 +612,9 @@
     <t>TX_16</t>
   </si>
   <si>
+    <t>Ask about activities that they do with others,PROMIS-29</t>
+  </si>
+  <si>
     <t>Testdata29</t>
   </si>
   <si>
@@ -645,6 +648,30 @@
     <t>ravikumar1@yopmail.com</t>
   </si>
   <si>
+    <t>Testdata33</t>
+  </si>
+  <si>
+    <t>Tx-testing1234</t>
+  </si>
+  <si>
+    <t>Sahil</t>
+  </si>
+  <si>
+    <t>kumar@yopmail.com</t>
+  </si>
+  <si>
+    <t>40</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>15</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
     <t>Testdata34</t>
   </si>
   <si>
@@ -654,6 +681,33 @@
     <t>Anita1</t>
   </si>
   <si>
+    <t>Testdata35</t>
+  </si>
+  <si>
+    <t>Tx-Testing9</t>
+  </si>
+  <si>
+    <t>Gita</t>
+  </si>
+  <si>
+    <t>15/OCT/2007</t>
+  </si>
+  <si>
+    <t>gita1@yopmail.com</t>
+  </si>
+  <si>
+    <t>30</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t>6.5</t>
+  </si>
+  <si>
+    <t>4.5</t>
+  </si>
+  <si>
     <t>Testdata36</t>
   </si>
   <si>
@@ -663,12 +717,6 @@
     <t>Raju</t>
   </si>
   <si>
-    <t>30</t>
-  </si>
-  <si>
-    <t>9</t>
-  </si>
-  <si>
     <t>8.5</t>
   </si>
   <si>
@@ -696,12 +744,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>6.5</t>
-  </si>
-  <si>
-    <t>4.5</t>
-  </si>
-  <si>
     <t>Testdata38</t>
   </si>
   <si>
@@ -714,6 +756,126 @@
     <t>7.5</t>
   </si>
   <si>
+    <t>Testdata39</t>
+  </si>
+  <si>
+    <t>Rahul</t>
+  </si>
+  <si>
+    <t>10/JAN/1999</t>
+  </si>
+  <si>
+    <t>42.5</t>
+  </si>
+  <si>
+    <t>12.5</t>
+  </si>
+  <si>
+    <t>13.5</t>
+  </si>
+  <si>
+    <t>Testdata40</t>
+  </si>
+  <si>
+    <t>Tx_Testing4</t>
+  </si>
+  <si>
+    <t>Raman</t>
+  </si>
+  <si>
+    <t>44</t>
+  </si>
+  <si>
+    <t>12</t>
+  </si>
+  <si>
+    <t>13</t>
+  </si>
+  <si>
+    <t>Testdata41</t>
+  </si>
+  <si>
+    <t>Tx-Testing8</t>
+  </si>
+  <si>
+    <t>Karan</t>
+  </si>
+  <si>
+    <t>125055</t>
+  </si>
+  <si>
+    <t>Rahul98@yopmail.com</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>Testdata42</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tx-Testing11</t>
+    </r>
+  </si>
+  <si>
+    <t>Singh</t>
+  </si>
+  <si>
+    <t>karan99@yopmail.com</t>
+  </si>
+  <si>
+    <t>1999</t>
+  </si>
+  <si>
+    <t>Testdata43</t>
+  </si>
+  <si>
+    <t>Tx-Testing15</t>
+  </si>
+  <si>
+    <t>Aman</t>
+  </si>
+  <si>
+    <t>Aman99@yopmail.com</t>
+  </si>
+  <si>
+    <t>Testdata44</t>
+  </si>
+  <si>
+    <t>Tx-Testing18</t>
+  </si>
+  <si>
+    <t>Amandeep</t>
+  </si>
+  <si>
+    <t>Testdata45</t>
+  </si>
+  <si>
+    <t>Tx_Testing3</t>
+  </si>
+  <si>
+    <t>Ramesh</t>
+  </si>
+  <si>
+    <t>1/JAN/2000</t>
+  </si>
+  <si>
+    <t>rameshsharma@yopmail.com</t>
+  </si>
+  <si>
+    <t>41.5</t>
+  </si>
+  <si>
+    <t>11.5</t>
+  </si>
+  <si>
     <t>Testdata46</t>
   </si>
   <si>
@@ -729,15 +891,6 @@
     <t>Ajay2reddy@yopmail.com</t>
   </si>
   <si>
-    <t>42.5</t>
-  </si>
-  <si>
-    <t>12.5</t>
-  </si>
-  <si>
-    <t>13.5</t>
-  </si>
-  <si>
     <t>Testdata47</t>
   </si>
   <si>
@@ -759,25 +912,37 @@
     <t>Tx-Testing10</t>
   </si>
   <si>
-    <t>Rahul</t>
-  </si>
-  <si>
-    <t>Rahul98@yopmail.com</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t>Testdata33</t>
-  </si>
-  <si>
-    <t>Sharma</t>
-  </si>
-  <si>
-    <t>Tx-Testing2201</t>
-  </si>
-  <si>
-    <t>Tx-Testing2422</t>
+    <t>Testdata49</t>
+  </si>
+  <si>
+    <t>Tx-Testing14</t>
+  </si>
+  <si>
+    <t>Lucky</t>
+  </si>
+  <si>
+    <t>luckysingh@yopmail.com</t>
+  </si>
+  <si>
+    <t>9/JUN/2012</t>
+  </si>
+  <si>
+    <t>Testdata50</t>
+  </si>
+  <si>
+    <t>Tx-Testing17</t>
+  </si>
+  <si>
+    <t>Ram</t>
+  </si>
+  <si>
+    <t>Thakur</t>
+  </si>
+  <si>
+    <t>ramthakur@yopmail.com</t>
+  </si>
+  <si>
+    <t>1/MAR/2014</t>
   </si>
 </sst>
 </file>
@@ -792,7 +957,7 @@
     <numFmt numFmtId="180" formatCode="dd/mmm/yy"/>
     <numFmt numFmtId="181" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -805,6 +970,35 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF454A4A"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <u/>
@@ -1349,134 +1543,134 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1488,6 +1682,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1501,17 +1699,24 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="181" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1779,22 +1984,22 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="13.5428571428571" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="49.4571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="26.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="11.0952380952381" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="33.1809523809524" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.6380952380952" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="19.7238095238095" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="64.2761904761905" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="28.1809523809524" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="102.180952380952" collapsed="true"/>
-    <col min="15" max="15" customWidth="true" width="19.9047619047619" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="26.6380952380952" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="30.5428571428571" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="25.8190476190476" collapsed="true"/>
+    <col min="1" max="1" width="13.5428571428571" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.4571428571429" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.0952380952381" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.1809523809524" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.6380952380952" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.7238095238095" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="64.2761904761905" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.1809523809524" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="102.180952380952" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.9047619047619" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.6380952380952" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.5428571428571" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="25.8190476190476" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="15" spans="1:18">
@@ -1922,7 +2127,7 @@
       <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="22" t="s">
+      <c r="L3" s="31" t="s">
         <v>30</v>
       </c>
     </row>
@@ -1998,7 +2203,7 @@
       <c r="K5" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="22" t="s">
+      <c r="L5" s="31" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2036,11 +2241,11 @@
       <c r="K6" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="L6" s="31" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="T6" s="22"/>
+      <c r="T6" s="31"/>
     </row>
     <row r="7" customHeight="1" spans="1:12">
       <c r="A7" t="s">
@@ -2108,7 +2313,7 @@
       <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K8" t="s">
@@ -2143,13 +2348,13 @@
       <c r="I9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K9" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="22" t="s">
+      <c r="L9" s="31" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2181,7 +2386,7 @@
       <c r="I10" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K10" t="s">
@@ -2216,7 +2421,7 @@
       <c r="I11" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K11" t="s">
@@ -2254,13 +2459,13 @@
       <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K12" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="31" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2292,13 +2497,13 @@
       <c r="I13" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K13" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="22" t="s">
+      <c r="L13" s="31" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2330,7 +2535,7 @@
       <c r="I14" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K14" t="s">
@@ -2409,7 +2614,7 @@
       <c r="K16" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="31" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2485,7 +2690,7 @@
       <c r="K18" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="22" t="s">
+      <c r="L18" s="31" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2523,7 +2728,7 @@
       <c r="K19" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="22" t="s">
+      <c r="L19" s="31" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2593,7 +2798,7 @@
       <c r="I21" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K21" t="s">
@@ -2611,7 +2816,7 @@
       <c r="O21" t="s">
         <v>63</v>
       </c>
-      <c r="P21" s="23" t="s">
+      <c r="P21" s="32" t="s">
         <v>64</v>
       </c>
       <c r="Q21" s="3" t="s">
@@ -2649,7 +2854,7 @@
       <c r="I22" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="32" t="s">
         <v>45</v>
       </c>
       <c r="K22" t="s">
@@ -2860,17 +3065,17 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="53.4571428571429" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="41.0952380952381" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="19.8190476190476" collapsed="true"/>
-    <col min="5" max="6" customWidth="true" width="24.5428571428571" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="30.8190476190476" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="14.2761904761905" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="35.4571428571429" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="41.4571428571429" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="27.8190476190476" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="16.4571428571429" collapsed="true"/>
+    <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.4571428571429" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.0952380952381" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.8190476190476" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="24.5428571428571" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.8190476190476" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.2761904761905" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="35.4571428571429" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="41.4571428571429" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.8190476190476" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.4571428571429" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -2971,13 +3176,13 @@
       <c r="H3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="20" t="s">
+      <c r="I3" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="20" t="s">
+      <c r="J3" s="29" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="20" t="s">
+      <c r="K3" s="29" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3012,7 +3217,7 @@
       <c r="J4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="28" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3026,7 +3231,7 @@
       <c r="C5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="19" t="s">
+      <c r="D5" s="28" t="s">
         <v>66</v>
       </c>
       <c r="E5" t="s">
@@ -3146,7 +3351,7 @@
       <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="33" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3322,36 +3527,36 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AB44"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="AA18" sqref="AA18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A45" sqref="A45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="16.4571428571429" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="52.8190476190476" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="38.9047619047619" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="18.2761904761905" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.4571428571429" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="17.6380952380952" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="41.1809523809524" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="22.3619047619048" collapsed="true"/>
-    <col min="9" max="9" customWidth="true" width="24.8190476190476" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="17.0" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="15.3619047619048" collapsed="true"/>
-    <col min="12" max="12" customWidth="true" width="26.6380952380952" collapsed="true"/>
-    <col min="13" max="13" customWidth="true" width="15.3619047619048" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" width="13.7238095238095" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="17.4571428571429" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="26.3619047619048" collapsed="true"/>
-    <col min="19" max="19" customWidth="true" width="23.5428571428571" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="18.7238095238095" collapsed="true"/>
-    <col min="21" max="21" customWidth="true" width="16.4571428571429" collapsed="true"/>
-    <col min="22" max="22" customWidth="true" width="13.0952380952381" collapsed="true"/>
-    <col min="23" max="23" customWidth="true" width="13.5428571428571" collapsed="true"/>
-    <col min="24" max="24" customWidth="true" width="13.9047619047619" collapsed="true"/>
+    <col min="1" max="1" width="16.4571428571429" customWidth="1"/>
+    <col min="2" max="2" width="52.8190476190476" customWidth="1"/>
+    <col min="3" max="3" width="38.9047619047619" customWidth="1"/>
+    <col min="4" max="4" width="18.2761904761905" customWidth="1"/>
+    <col min="5" max="5" width="23.4571428571429" customWidth="1"/>
+    <col min="6" max="6" width="17.6380952380952" customWidth="1"/>
+    <col min="7" max="7" width="41.1809523809524" customWidth="1"/>
+    <col min="8" max="8" width="22.3619047619048" customWidth="1"/>
+    <col min="9" max="9" width="24.8190476190476" customWidth="1"/>
+    <col min="10" max="10" width="17" customWidth="1"/>
+    <col min="11" max="11" width="15.3619047619048" customWidth="1"/>
+    <col min="12" max="12" width="26.6380952380952" customWidth="1"/>
+    <col min="13" max="13" width="15.3619047619048" customWidth="1"/>
+    <col min="14" max="14" width="13.7238095238095" customWidth="1"/>
+    <col min="16" max="16" width="17.4571428571429" customWidth="1"/>
+    <col min="18" max="18" width="26.3619047619048" customWidth="1"/>
+    <col min="19" max="19" width="23.5428571428571" customWidth="1"/>
+    <col min="20" max="20" width="18.7238095238095" customWidth="1"/>
+    <col min="21" max="21" width="16.4571428571429" customWidth="1"/>
+    <col min="22" max="22" width="13.0952380952381" customWidth="1"/>
+    <col min="23" max="23" width="13.5428571428571" customWidth="1"/>
+    <col min="24" max="24" width="13.9047619047619" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:28">
@@ -3564,16 +3769,16 @@
       <c r="L5" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="M5" s="9" t="s">
+      <c r="M5" s="13" t="s">
         <v>128</v>
       </c>
       <c r="N5" t="s">
         <v>129</v>
       </c>
-      <c r="O5" s="9" t="s">
+      <c r="O5" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="P5" s="10" t="s">
+      <c r="P5" s="14" t="s">
         <v>131</v>
       </c>
       <c r="Q5" t="s">
@@ -3617,16 +3822,16 @@
       <c r="L6" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="M6" s="9" t="s">
+      <c r="M6" s="13" t="s">
         <v>128</v>
       </c>
       <c r="N6" t="s">
         <v>129</v>
       </c>
-      <c r="O6" s="9" t="s">
+      <c r="O6" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="P6" s="10" t="s">
+      <c r="P6" s="14" t="s">
         <v>131</v>
       </c>
       <c r="Q6" t="s">
@@ -3670,16 +3875,16 @@
       <c r="L7" s="3" t="s">
         <v>127</v>
       </c>
-      <c r="M7" s="9" t="s">
+      <c r="M7" s="13" t="s">
         <v>128</v>
       </c>
       <c r="N7" t="s">
         <v>129</v>
       </c>
-      <c r="O7" s="9" t="s">
+      <c r="O7" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="P7" s="10" t="s">
+      <c r="P7" s="14" t="s">
         <v>131</v>
       </c>
       <c r="Q7" t="s">
@@ -3723,8 +3928,8 @@
       <c r="L8" t="s">
         <v>129</v>
       </c>
-      <c r="M8" s="9"/>
-      <c r="N8" s="10" t="s">
+      <c r="M8" s="13"/>
+      <c r="N8" s="14" t="s">
         <v>131</v>
       </c>
       <c r="O8" t="s">
@@ -3742,7 +3947,7 @@
       <c r="S8" t="s">
         <v>124</v>
       </c>
-      <c r="T8" s="16" t="s">
+      <c r="T8" s="23" t="s">
         <v>135</v>
       </c>
     </row>
@@ -3807,16 +4012,16 @@
       <c r="L10" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="M10" s="9" t="s">
+      <c r="M10" s="13" t="s">
         <v>128</v>
       </c>
       <c r="N10" t="s">
         <v>129</v>
       </c>
-      <c r="O10" s="9" t="s">
+      <c r="O10" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="P10" s="10" t="s">
+      <c r="P10" s="14" t="s">
         <v>131</v>
       </c>
       <c r="Q10" t="s">
@@ -3869,7 +4074,7 @@
       <c r="O11">
         <v>1122</v>
       </c>
-      <c r="P11" s="11">
+      <c r="P11" s="15">
         <v>29749</v>
       </c>
       <c r="Q11" t="s">
@@ -4024,7 +4229,7 @@
       <c r="L15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="M15" s="12" t="s">
+      <c r="M15" s="16" t="s">
         <v>155</v>
       </c>
       <c r="N15" s="7" t="s">
@@ -4033,7 +4238,7 @@
       <c r="O15" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="P15" s="13" t="s">
+      <c r="P15" s="17" t="s">
         <v>156</v>
       </c>
       <c r="Q15" s="7" t="s">
@@ -4150,16 +4355,16 @@
       <c r="L18" t="s">
         <v>165</v>
       </c>
-      <c r="M18" s="14" t="s">
+      <c r="M18" s="18" t="s">
         <v>166</v>
       </c>
       <c r="N18" t="s">
         <v>129</v>
       </c>
-      <c r="O18" s="14" t="s">
+      <c r="O18" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="P18" s="15" t="s">
+      <c r="P18" s="19" t="s">
         <v>168</v>
       </c>
       <c r="Q18" t="s">
@@ -4195,7 +4400,7 @@
       <c r="AA18" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="AB18" s="18" t="s">
+      <c r="AB18" s="4" t="s">
         <v>21</v>
       </c>
     </row>
@@ -4216,7 +4421,7 @@
         <v>171</v>
       </c>
       <c r="F19" t="s">
-        <v>238</v>
+        <v>172</v>
       </c>
       <c r="G19" t="s">
         <v>63</v>
@@ -4236,16 +4441,16 @@
       <c r="L19" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="M19" s="14" t="s">
+      <c r="M19" s="18" t="s">
         <v>176</v>
       </c>
       <c r="N19" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="O19" s="14" t="s">
+      <c r="O19" s="18" t="s">
         <v>167</v>
       </c>
-      <c r="P19" s="15" t="s">
+      <c r="P19" s="19" t="s">
         <v>131</v>
       </c>
       <c r="Q19" s="8" t="s">
@@ -4381,9 +4586,9 @@
         <v>180</v>
       </c>
     </row>
-    <row r="23" spans="1:7">
-      <c r="A23" s="7" t="s">
-        <v>183</v>
+    <row r="23" spans="1:28">
+      <c r="A23" t="s">
+        <v>67</v>
       </c>
       <c r="B23" s="3" t="s">
         <v>19</v>
@@ -4394,19 +4599,82 @@
       <c r="D23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E23" s="6" t="s">
+      <c r="E23" t="s">
+        <v>164</v>
+      </c>
+      <c r="F23" t="s">
+        <v>133</v>
+      </c>
+      <c r="G23" t="s">
+        <v>63</v>
+      </c>
+      <c r="H23" t="s">
+        <v>63</v>
+      </c>
+      <c r="I23" t="s">
+        <v>63</v>
+      </c>
+      <c r="J23" t="s">
+        <v>150</v>
+      </c>
+      <c r="K23" t="s">
+        <v>151</v>
+      </c>
+      <c r="L23" t="s">
+        <v>165</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="N23" t="s">
+        <v>129</v>
+      </c>
+      <c r="O23" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="P23" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>132</v>
+      </c>
+      <c r="R23" t="s">
+        <v>63</v>
+      </c>
+      <c r="S23" t="s">
+        <v>63</v>
+      </c>
+      <c r="T23" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" t="s">
+        <v>63</v>
+      </c>
+      <c r="V23" t="s">
+        <v>63</v>
+      </c>
+      <c r="W23" t="s">
+        <v>63</v>
+      </c>
+      <c r="X23" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA23" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB23" s="27" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="7" t="s">
         <v>184</v>
-      </c>
-      <c r="F23" t="s">
-        <v>185</v>
-      </c>
-      <c r="G23" s="7" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="24" spans="1:25">
-      <c r="A24" s="7" t="s">
-        <v>186</v>
       </c>
       <c r="B24" s="3" t="s">
         <v>19</v>
@@ -4418,59 +4686,18 @@
         <v>21</v>
       </c>
       <c r="E24" s="6" t="s">
+        <v>185</v>
+      </c>
+      <c r="F24" t="s">
+        <v>186</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25">
+      <c r="A25" s="7" t="s">
         <v>187</v>
-      </c>
-      <c r="F24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="I24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="J24" s="6" t="s">
-        <v>180</v>
-      </c>
-      <c r="K24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M24" s="12">
-        <v>500018</v>
-      </c>
-      <c r="N24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P24" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q24" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R24" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="S24" s="6" t="s">
-        <v>189</v>
-      </c>
-      <c r="U24" s="10"/>
-      <c r="V24" s="10"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="10"/>
-      <c r="Y24" s="10"/>
-    </row>
-    <row r="25" spans="1:19">
-      <c r="A25" s="7" t="s">
-        <v>190</v>
       </c>
       <c r="B25" s="3" t="s">
         <v>19</v>
@@ -4482,10 +4709,22 @@
         <v>21</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>191</v>
+        <v>188</v>
+      </c>
+      <c r="F25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="H25" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="I25" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="J25" s="6" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="K25" s="7" t="s">
         <v>63</v>
@@ -4493,8 +4732,8 @@
       <c r="L25" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="M25" s="12" t="s">
-        <v>155</v>
+      <c r="M25" s="16">
+        <v>500018</v>
       </c>
       <c r="N25" s="7" t="s">
         <v>63</v>
@@ -4502,8 +4741,8 @@
       <c r="O25" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="P25" s="13" t="s">
-        <v>188</v>
+      <c r="P25" s="17" t="s">
+        <v>189</v>
       </c>
       <c r="Q25" s="7" t="s">
         <v>63</v>
@@ -4511,13 +4750,18 @@
       <c r="R25" s="7" t="s">
         <v>157</v>
       </c>
-      <c r="S25" s="4" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10">
+      <c r="S25" s="6" t="s">
+        <v>190</v>
+      </c>
+      <c r="U25" s="14"/>
+      <c r="V25" s="14"/>
+      <c r="W25" s="14"/>
+      <c r="X25" s="14"/>
+      <c r="Y25" s="14"/>
+    </row>
+    <row r="26" spans="1:19">
       <c r="A26" s="7" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>19</v>
@@ -4529,18 +4773,42 @@
         <v>21</v>
       </c>
       <c r="E26" s="6" t="s">
+        <v>192</v>
+      </c>
+      <c r="J26" s="6" t="s">
+        <v>193</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P26" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S26" s="4" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28">
+      <c r="A27" t="s">
         <v>195</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>196</v>
-      </c>
-      <c r="J26" s="6" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="27" spans="1:25">
-      <c r="A27" s="7" t="s">
-        <v>197</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>19</v>
@@ -4551,73 +4819,82 @@
       <c r="D27" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E27" s="6" t="s">
+      <c r="E27" t="s">
+        <v>196</v>
+      </c>
+      <c r="F27" t="s">
+        <v>63</v>
+      </c>
+      <c r="G27" t="s">
+        <v>63</v>
+      </c>
+      <c r="H27" t="s">
+        <v>63</v>
+      </c>
+      <c r="I27" t="s">
+        <v>63</v>
+      </c>
+      <c r="J27" t="s">
+        <v>197</v>
+      </c>
+      <c r="K27" t="s">
+        <v>126</v>
+      </c>
+      <c r="L27" t="s">
         <v>198</v>
       </c>
-      <c r="F27" t="s">
-        <v>63</v>
-      </c>
-      <c r="G27" t="s">
-        <v>63</v>
-      </c>
-      <c r="H27" t="s">
-        <v>63</v>
-      </c>
-      <c r="I27" t="s">
-        <v>63</v>
-      </c>
-      <c r="J27" s="6" t="s">
+      <c r="M27" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="N27" t="s">
+        <v>129</v>
+      </c>
+      <c r="O27" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="P27" s="19" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q27" t="s">
+        <v>132</v>
+      </c>
+      <c r="R27" t="s">
+        <v>63</v>
+      </c>
+      <c r="S27" t="s">
+        <v>63</v>
+      </c>
+      <c r="T27" t="s">
+        <v>63</v>
+      </c>
+      <c r="U27" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="K27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="S27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="T27" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="U27" s="10" t="s">
+      <c r="V27" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="V27" s="10" t="s">
+      <c r="W27" s="17" t="s">
         <v>201</v>
       </c>
-      <c r="W27" s="10" t="s">
-        <v>201</v>
-      </c>
-      <c r="X27" s="10" t="s">
+      <c r="X27" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y27" s="17" t="s">
         <v>202</v>
       </c>
-      <c r="Y27" s="10" t="s">
+      <c r="Z27" t="s">
+        <v>183</v>
+      </c>
+      <c r="AA27" t="s">
+        <v>20</v>
+      </c>
+      <c r="AB27" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10">
+      <c r="A28" s="7" t="s">
         <v>203</v>
-      </c>
-    </row>
-    <row r="28" spans="1:25">
-      <c r="A28" s="7" t="s">
-        <v>204</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>19</v>
@@ -4629,72 +4906,18 @@
         <v>21</v>
       </c>
       <c r="E28" s="6" t="s">
+        <v>204</v>
+      </c>
+      <c r="F28" s="6" t="s">
         <v>205</v>
       </c>
-      <c r="F28" t="s">
-        <v>63</v>
-      </c>
-      <c r="G28" t="s">
-        <v>63</v>
-      </c>
-      <c r="H28" t="s">
-        <v>63</v>
-      </c>
-      <c r="I28" t="s">
-        <v>63</v>
-      </c>
       <c r="J28" s="6" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28">
+      <c r="A29" t="s">
         <v>206</v>
-      </c>
-      <c r="K28" t="s">
-        <v>63</v>
-      </c>
-      <c r="L28" t="s">
-        <v>63</v>
-      </c>
-      <c r="M28" s="12" t="s">
-        <v>207</v>
-      </c>
-      <c r="N28" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O28" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P28" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q28" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R28" t="s">
-        <v>157</v>
-      </c>
-      <c r="S28" s="4" t="s">
-        <v>208</v>
-      </c>
-      <c r="T28" t="s">
-        <v>63</v>
-      </c>
-      <c r="U28" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="V28" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="W28" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="X28" s="10" t="s">
-        <v>211</v>
-      </c>
-      <c r="Y28" s="10" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="29" spans="1:25">
-      <c r="A29" s="7" t="s">
-        <v>213</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>19</v>
@@ -4705,73 +4928,82 @@
       <c r="D29" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E29" s="6" t="s">
+      <c r="E29" t="s">
+        <v>207</v>
+      </c>
+      <c r="F29" t="s">
+        <v>63</v>
+      </c>
+      <c r="G29" t="s">
+        <v>63</v>
+      </c>
+      <c r="H29" t="s">
+        <v>63</v>
+      </c>
+      <c r="I29" t="s">
+        <v>63</v>
+      </c>
+      <c r="J29" t="s">
+        <v>208</v>
+      </c>
+      <c r="K29" t="s">
+        <v>63</v>
+      </c>
+      <c r="L29" t="s">
+        <v>63</v>
+      </c>
+      <c r="M29" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="N29" t="s">
+        <v>63</v>
+      </c>
+      <c r="O29" t="s">
+        <v>63</v>
+      </c>
+      <c r="P29" s="19" t="s">
+        <v>209</v>
+      </c>
+      <c r="Q29" t="s">
+        <v>63</v>
+      </c>
+      <c r="R29" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S29" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="T29" t="s">
+        <v>63</v>
+      </c>
+      <c r="U29" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V29" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="W29" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="X29" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y29" s="17" t="s">
         <v>214</v>
       </c>
-      <c r="F29" t="s">
-        <v>63</v>
-      </c>
-      <c r="G29" t="s">
-        <v>63</v>
-      </c>
-      <c r="H29" t="s">
-        <v>63</v>
-      </c>
-      <c r="I29" t="s">
-        <v>63</v>
-      </c>
-      <c r="J29" s="6" t="s">
-        <v>215</v>
-      </c>
-      <c r="K29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="N29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="S29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="T29" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="U29" s="13" t="s">
-        <v>200</v>
-      </c>
-      <c r="V29" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="W29" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="X29" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y29" s="13" t="s">
-        <v>212</v>
+      <c r="Z29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA29" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB29" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="30" spans="1:25">
       <c r="A30" s="7" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>19</v>
@@ -4783,72 +5015,72 @@
         <v>21</v>
       </c>
       <c r="E30" s="6" t="s">
+        <v>216</v>
+      </c>
+      <c r="F30" t="s">
+        <v>63</v>
+      </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s">
+        <v>63</v>
+      </c>
+      <c r="I30" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" s="6" t="s">
+        <v>217</v>
+      </c>
+      <c r="K30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T30" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U30" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V30" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="W30" s="14" t="s">
+        <v>212</v>
+      </c>
+      <c r="X30" s="14" t="s">
         <v>218</v>
       </c>
-      <c r="F30" t="s">
-        <v>63</v>
-      </c>
-      <c r="G30" t="s">
-        <v>63</v>
-      </c>
-      <c r="H30" t="s">
-        <v>63</v>
-      </c>
-      <c r="I30" t="s">
-        <v>63</v>
-      </c>
-      <c r="J30" s="6" t="s">
+      <c r="Y30" s="14" t="s">
         <v>219</v>
-      </c>
-      <c r="K30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M30" s="12" t="s">
-        <v>220</v>
-      </c>
-      <c r="N30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P30" s="13" t="s">
-        <v>188</v>
-      </c>
-      <c r="Q30" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R30" t="s">
-        <v>157</v>
-      </c>
-      <c r="S30" s="6" t="s">
-        <v>221</v>
-      </c>
-      <c r="T30" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="U30" s="13" t="s">
-        <v>222</v>
-      </c>
-      <c r="V30" s="13" t="s">
-        <v>223</v>
-      </c>
-      <c r="W30" s="13" t="s">
-        <v>224</v>
-      </c>
-      <c r="X30" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="Y30" s="13" t="s">
-        <v>216</v>
       </c>
     </row>
     <row r="31" spans="1:25">
       <c r="A31" s="7" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>19</v>
@@ -4860,7 +5092,7 @@
         <v>21</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="F31" t="s">
         <v>63</v>
@@ -4875,16 +5107,16 @@
         <v>63</v>
       </c>
       <c r="J31" s="6" t="s">
-        <v>227</v>
-      </c>
-      <c r="K31" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="L31" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M31" s="12" t="s">
-        <v>176</v>
+        <v>222</v>
+      </c>
+      <c r="K31" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" t="s">
+        <v>63</v>
+      </c>
+      <c r="M31" s="16" t="s">
+        <v>223</v>
       </c>
       <c r="N31" s="7" t="s">
         <v>63</v>
@@ -4892,8 +5124,8 @@
       <c r="O31" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="P31" s="13" t="s">
-        <v>228</v>
+      <c r="P31" s="17" t="s">
+        <v>189</v>
       </c>
       <c r="Q31" s="7" t="s">
         <v>63</v>
@@ -4901,31 +5133,31 @@
       <c r="R31" t="s">
         <v>157</v>
       </c>
-      <c r="S31" s="6" t="s">
-        <v>229</v>
-      </c>
-      <c r="T31" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="U31" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="V31" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="W31" s="13" t="s">
-        <v>201</v>
-      </c>
-      <c r="X31" s="13" t="s">
-        <v>202</v>
-      </c>
-      <c r="Y31" s="13" t="s">
-        <v>203</v>
+      <c r="S31" s="4" t="s">
+        <v>224</v>
+      </c>
+      <c r="T31" t="s">
+        <v>63</v>
+      </c>
+      <c r="U31" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V31" s="14" t="s">
+        <v>225</v>
+      </c>
+      <c r="W31" s="14" t="s">
+        <v>226</v>
+      </c>
+      <c r="X31" s="14" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y31" s="14" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="32" spans="1:25">
       <c r="A32" s="7" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>19</v>
@@ -4937,9 +5169,9 @@
         <v>21</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>231</v>
-      </c>
-      <c r="F32" s="6" t="s">
+        <v>228</v>
+      </c>
+      <c r="F32" t="s">
         <v>63</v>
       </c>
       <c r="G32" t="s">
@@ -4952,7 +5184,7 @@
         <v>63</v>
       </c>
       <c r="J32" s="6" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="K32" s="7" t="s">
         <v>63</v>
@@ -4960,8 +5192,8 @@
       <c r="L32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="M32" s="12" t="s">
-        <v>166</v>
+      <c r="M32" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="N32" s="7" t="s">
         <v>63</v>
@@ -4969,40 +5201,40 @@
       <c r="O32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="P32" s="13" t="s">
-        <v>131</v>
+      <c r="P32" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="Q32" s="7" t="s">
         <v>63</v>
       </c>
       <c r="R32" s="7" t="s">
-        <v>157</v>
-      </c>
-      <c r="S32" s="17" t="s">
-        <v>233</v>
+        <v>63</v>
+      </c>
+      <c r="S32" s="7" t="s">
+        <v>63</v>
       </c>
       <c r="T32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="U32" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="V32" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="W32" s="13" t="s">
-        <v>234</v>
-      </c>
-      <c r="X32" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y32" s="13" t="s">
+      <c r="U32" s="17" t="s">
+        <v>211</v>
+      </c>
+      <c r="V32" s="17" t="s">
         <v>212</v>
+      </c>
+      <c r="W32" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="X32" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y32" s="17" t="s">
+        <v>214</v>
       </c>
     </row>
     <row r="33" spans="1:25">
       <c r="A33" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>19</v>
@@ -5013,10 +5245,10 @@
       <c r="D33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="E33" s="6" t="s">
+      <c r="E33" t="s">
         <v>164</v>
       </c>
-      <c r="F33" s="6" t="s">
+      <c r="F33" t="s">
         <v>63</v>
       </c>
       <c r="G33" t="s">
@@ -5032,49 +5264,932 @@
         <v>232</v>
       </c>
       <c r="K33" t="s">
+        <v>63</v>
+      </c>
+      <c r="L33" t="s">
+        <v>63</v>
+      </c>
+      <c r="M33" s="14" t="s">
+        <v>166</v>
+      </c>
+      <c r="N33" t="s">
+        <v>63</v>
+      </c>
+      <c r="O33" t="s">
+        <v>63</v>
+      </c>
+      <c r="P33" s="14" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>63</v>
+      </c>
+      <c r="R33" t="s">
+        <v>63</v>
+      </c>
+      <c r="S33" t="s">
+        <v>63</v>
+      </c>
+      <c r="T33" t="s">
+        <v>63</v>
+      </c>
+      <c r="U33" s="14" t="s">
+        <v>234</v>
+      </c>
+      <c r="V33" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="W33" s="17" t="s">
         <v>236</v>
       </c>
-      <c r="L33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="M33" s="12" t="s">
+      <c r="X33" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="Y33" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25">
+      <c r="A34" t="s">
+        <v>237</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C34" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E34" t="s">
+        <v>238</v>
+      </c>
+      <c r="F34" t="s">
+        <v>63</v>
+      </c>
+      <c r="G34" t="s">
+        <v>63</v>
+      </c>
+      <c r="H34" t="s">
+        <v>63</v>
+      </c>
+      <c r="I34" t="s">
+        <v>63</v>
+      </c>
+      <c r="J34" t="s">
+        <v>239</v>
+      </c>
+      <c r="K34" t="s">
+        <v>63</v>
+      </c>
+      <c r="L34" t="s">
+        <v>63</v>
+      </c>
+      <c r="M34" s="14" t="s">
         <v>166</v>
       </c>
-      <c r="N33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="O33" s="9" t="s">
-        <v>167</v>
-      </c>
-      <c r="P33" s="13" t="s">
+      <c r="N34" t="s">
+        <v>63</v>
+      </c>
+      <c r="O34" t="s">
+        <v>63</v>
+      </c>
+      <c r="P34" s="14" t="s">
+        <v>168</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>63</v>
+      </c>
+      <c r="R34" t="s">
+        <v>63</v>
+      </c>
+      <c r="S34" t="s">
+        <v>63</v>
+      </c>
+      <c r="T34" t="s">
+        <v>63</v>
+      </c>
+      <c r="U34" s="14" t="s">
+        <v>240</v>
+      </c>
+      <c r="V34" s="17" t="s">
+        <v>241</v>
+      </c>
+      <c r="W34" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="X34" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y34" s="17" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25">
+      <c r="A35" s="9" t="s">
+        <v>243</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C35" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D35" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E35" s="12" t="s">
+        <v>244</v>
+      </c>
+      <c r="F35" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G35" t="s">
+        <v>63</v>
+      </c>
+      <c r="H35" t="s">
+        <v>63</v>
+      </c>
+      <c r="I35" t="s">
+        <v>63</v>
+      </c>
+      <c r="J35" t="s">
+        <v>245</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="L35" t="s">
+        <v>63</v>
+      </c>
+      <c r="M35" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="N35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O35" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P35" s="14" t="s">
         <v>131</v>
       </c>
-      <c r="Q33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="R33" s="7" t="s">
+      <c r="Q35" t="s">
+        <v>63</v>
+      </c>
+      <c r="R35" t="s">
         <v>157</v>
       </c>
-      <c r="S33" s="17" t="s">
+      <c r="S35" s="25" t="s">
+        <v>247</v>
+      </c>
+      <c r="T35" t="s">
+        <v>63</v>
+      </c>
+      <c r="U35" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V35" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="W35" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="X35" s="21" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y35" s="21" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="36" spans="1:28">
+      <c r="A36" t="s">
+        <v>249</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E36" t="s">
+        <v>250</v>
+      </c>
+      <c r="F36" t="s">
+        <v>63</v>
+      </c>
+      <c r="G36" t="s">
+        <v>63</v>
+      </c>
+      <c r="H36" t="s">
+        <v>63</v>
+      </c>
+      <c r="I36" t="s">
+        <v>63</v>
+      </c>
+      <c r="J36" t="s">
+        <v>245</v>
+      </c>
+      <c r="K36" t="s">
+        <v>251</v>
+      </c>
+      <c r="L36" t="s">
+        <v>252</v>
+      </c>
+      <c r="M36" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="N36" t="s">
+        <v>129</v>
+      </c>
+      <c r="O36" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="P36" s="19" t="s">
         <v>233</v>
       </c>
-      <c r="T33" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="U33" s="10" t="s">
+      <c r="Q36" t="s">
+        <v>132</v>
+      </c>
+      <c r="R36" t="s">
+        <v>157</v>
+      </c>
+      <c r="S36" t="s">
+        <v>252</v>
+      </c>
+      <c r="T36" t="s">
+        <v>63</v>
+      </c>
+      <c r="U36" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V36" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="W36" s="17" t="s">
         <v>200</v>
       </c>
-      <c r="V33" s="13" t="s">
-        <v>209</v>
-      </c>
-      <c r="W33" s="13" t="s">
+      <c r="X36" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y36" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25">
+      <c r="A37" s="9" t="s">
+        <v>254</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C37" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D37" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="E37" s="12" t="s">
+        <v>255</v>
+      </c>
+      <c r="F37" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G37" t="s">
+        <v>63</v>
+      </c>
+      <c r="H37" t="s">
+        <v>63</v>
+      </c>
+      <c r="I37" t="s">
+        <v>63</v>
+      </c>
+      <c r="J37" s="12" t="s">
+        <v>256</v>
+      </c>
+      <c r="K37" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L37" t="s">
+        <v>63</v>
+      </c>
+      <c r="M37" s="20" t="s">
+        <v>246</v>
+      </c>
+      <c r="N37" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O37" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P37" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>63</v>
+      </c>
+      <c r="R37" t="s">
+        <v>157</v>
+      </c>
+      <c r="S37" s="12" t="s">
+        <v>257</v>
+      </c>
+      <c r="T37" t="s">
+        <v>63</v>
+      </c>
+      <c r="U37" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V37" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="W37" s="21" t="s">
+        <v>212</v>
+      </c>
+      <c r="X37" s="14" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y37" s="14" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="38" spans="1:28">
+      <c r="A38" t="s">
+        <v>258</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E38" t="s">
+        <v>259</v>
+      </c>
+      <c r="F38" t="s">
+        <v>63</v>
+      </c>
+      <c r="G38" t="s">
+        <v>63</v>
+      </c>
+      <c r="H38" t="s">
+        <v>63</v>
+      </c>
+      <c r="I38" t="s">
+        <v>63</v>
+      </c>
+      <c r="J38" t="s">
+        <v>260</v>
+      </c>
+      <c r="K38" t="s">
+        <v>63</v>
+      </c>
+      <c r="L38" t="s">
+        <v>63</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>246</v>
+      </c>
+      <c r="N38" t="s">
+        <v>63</v>
+      </c>
+      <c r="O38" t="s">
+        <v>63</v>
+      </c>
+      <c r="P38" s="19" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>63</v>
+      </c>
+      <c r="R38" t="s">
+        <v>63</v>
+      </c>
+      <c r="S38" t="s">
+        <v>63</v>
+      </c>
+      <c r="T38" t="s">
+        <v>63</v>
+      </c>
+      <c r="U38" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V38" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="W38" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="X38" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y38" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA38" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB38" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25">
+      <c r="A39" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="B39" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="E39" s="12" t="s">
+        <v>262</v>
+      </c>
+      <c r="F39" t="s">
+        <v>63</v>
+      </c>
+      <c r="G39" t="s">
+        <v>63</v>
+      </c>
+      <c r="H39" t="s">
+        <v>63</v>
+      </c>
+      <c r="I39" t="s">
+        <v>63</v>
+      </c>
+      <c r="J39" t="s">
+        <v>263</v>
+      </c>
+      <c r="K39" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L39" t="s">
+        <v>63</v>
+      </c>
+      <c r="M39" s="20" t="s">
+        <v>176</v>
+      </c>
+      <c r="N39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="O39" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="P39" s="21" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>63</v>
+      </c>
+      <c r="R39" t="s">
+        <v>157</v>
+      </c>
+      <c r="S39" t="s">
+        <v>265</v>
+      </c>
+      <c r="T39" t="s">
+        <v>63</v>
+      </c>
+      <c r="U39" s="14" t="s">
+        <v>266</v>
+      </c>
+      <c r="V39" s="14" t="s">
+        <v>267</v>
+      </c>
+      <c r="W39" s="14" t="s">
+        <v>236</v>
+      </c>
+      <c r="X39" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y39" s="14" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="40" spans="1:25">
+      <c r="A40" s="7" t="s">
+        <v>268</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E40" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="F40" t="s">
+        <v>63</v>
+      </c>
+      <c r="G40" t="s">
+        <v>63</v>
+      </c>
+      <c r="H40" t="s">
+        <v>63</v>
+      </c>
+      <c r="I40" t="s">
+        <v>63</v>
+      </c>
+      <c r="J40" s="6" t="s">
+        <v>270</v>
+      </c>
+      <c r="K40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M40" s="16" t="s">
+        <v>271</v>
+      </c>
+      <c r="N40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P40" s="17" t="s">
+        <v>189</v>
+      </c>
+      <c r="Q40" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R40" t="s">
+        <v>157</v>
+      </c>
+      <c r="S40" s="6" t="s">
+        <v>272</v>
+      </c>
+      <c r="T40" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="U40" s="17" t="s">
         <v>234</v>
       </c>
-      <c r="X33" s="13" t="s">
-        <v>216</v>
-      </c>
-      <c r="Y33" s="13" t="s">
+      <c r="V40" s="17" t="s">
+        <v>235</v>
+      </c>
+      <c r="W40" s="17" t="s">
+        <v>236</v>
+      </c>
+      <c r="X40" s="17" t="s">
         <v>212</v>
+      </c>
+      <c r="Y40" s="17" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="41" spans="1:25">
+      <c r="A41" s="7" t="s">
+        <v>273</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E41" s="6" t="s">
+        <v>274</v>
+      </c>
+      <c r="F41" t="s">
+        <v>63</v>
+      </c>
+      <c r="G41" t="s">
+        <v>63</v>
+      </c>
+      <c r="H41" t="s">
+        <v>63</v>
+      </c>
+      <c r="I41" t="s">
+        <v>63</v>
+      </c>
+      <c r="J41" s="6" t="s">
+        <v>275</v>
+      </c>
+      <c r="K41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M41" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="N41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P41" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="Q41" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R41" t="s">
+        <v>157</v>
+      </c>
+      <c r="S41" s="6" t="s">
+        <v>277</v>
+      </c>
+      <c r="T41" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="U41" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V41" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="W41" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="X41" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y41" s="17" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="42" spans="1:25">
+      <c r="A42" s="7" t="s">
+        <v>278</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D42" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E42" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="F42" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="G42" t="s">
+        <v>63</v>
+      </c>
+      <c r="H42" t="s">
+        <v>63</v>
+      </c>
+      <c r="I42" t="s">
+        <v>63</v>
+      </c>
+      <c r="J42" s="6" t="s">
+        <v>232</v>
+      </c>
+      <c r="K42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M42" s="16" t="s">
+        <v>166</v>
+      </c>
+      <c r="N42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P42" s="17" t="s">
+        <v>131</v>
+      </c>
+      <c r="Q42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R42" s="7" t="s">
+        <v>157</v>
+      </c>
+      <c r="S42" s="26" t="s">
+        <v>247</v>
+      </c>
+      <c r="T42" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U42" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V42" s="17" t="s">
+        <v>225</v>
+      </c>
+      <c r="W42" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="X42" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="Y42" s="17" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="43" spans="1:28">
+      <c r="A43" t="s">
+        <v>280</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" t="s">
+        <v>281</v>
+      </c>
+      <c r="F43" t="s">
+        <v>63</v>
+      </c>
+      <c r="G43" t="s">
+        <v>63</v>
+      </c>
+      <c r="H43" t="s">
+        <v>63</v>
+      </c>
+      <c r="I43" t="s">
+        <v>63</v>
+      </c>
+      <c r="J43" t="s">
+        <v>282</v>
+      </c>
+      <c r="K43" t="s">
+        <v>251</v>
+      </c>
+      <c r="L43" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="M43" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="N43" t="s">
+        <v>129</v>
+      </c>
+      <c r="O43" s="18" t="s">
+        <v>253</v>
+      </c>
+      <c r="P43" s="19" t="s">
+        <v>284</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>132</v>
+      </c>
+      <c r="R43" t="s">
+        <v>157</v>
+      </c>
+      <c r="S43" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="T43" t="s">
+        <v>63</v>
+      </c>
+      <c r="U43" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V43" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="W43" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="X43" s="17" t="s">
+        <v>213</v>
+      </c>
+      <c r="Y43" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA43" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:28">
+      <c r="A44" t="s">
+        <v>285</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D44" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E44" t="s">
+        <v>286</v>
+      </c>
+      <c r="F44" t="s">
+        <v>63</v>
+      </c>
+      <c r="G44" t="s">
+        <v>63</v>
+      </c>
+      <c r="H44" t="s">
+        <v>63</v>
+      </c>
+      <c r="I44" t="s">
+        <v>63</v>
+      </c>
+      <c r="J44" t="s">
+        <v>287</v>
+      </c>
+      <c r="K44" t="s">
+        <v>288</v>
+      </c>
+      <c r="L44" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="M44" s="18" t="s">
+        <v>176</v>
+      </c>
+      <c r="N44" t="s">
+        <v>129</v>
+      </c>
+      <c r="O44" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="P44" s="19" t="s">
+        <v>290</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>132</v>
+      </c>
+      <c r="R44" t="s">
+        <v>157</v>
+      </c>
+      <c r="S44" s="22" t="s">
+        <v>289</v>
+      </c>
+      <c r="T44" t="s">
+        <v>63</v>
+      </c>
+      <c r="U44" s="14" t="s">
+        <v>211</v>
+      </c>
+      <c r="V44" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="W44" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="X44" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="Y44" s="17" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>63</v>
       </c>
     </row>
   </sheetData>
@@ -5133,25 +6248,15 @@
     <hyperlink ref="C11" r:id="rId9" display="dhanya@yopmail.com"/>
     <hyperlink ref="L11" r:id="rId10" display="shardha@yopmail.com"/>
     <hyperlink ref="B12" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="B23" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D23" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C23" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="B25" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D25" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C25" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B24" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D24" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C24" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B26" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D26" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C26" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="B27" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D27" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C27" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B28" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D28" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C28" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="B29" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D29" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C29" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="S28" r:id="rId11" display="ajay@yopmail.com"/>
     <hyperlink ref="B30" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D30" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C30" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
@@ -5159,14 +6264,18 @@
     <hyperlink ref="D31" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C31" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B32" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D32" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C32" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="D32" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="B24" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="C24" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="D24" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="B33" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="C33" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="D33" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="S31" r:id="rId11" display="ajay@yopmail.com"/>
+    <hyperlink ref="B41" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D41" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C41" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B42" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C42" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D42" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="B25" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C25" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D25" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="D18" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C18" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B18" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
@@ -5176,6 +6285,51 @@
     <hyperlink ref="C19" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="D19" r:id="rId12" display="Sah@6057" tooltip="mailto:Sah@6057"/>
     <hyperlink ref="L19" r:id="rId13" display="preet98@yopmail.com" tooltip="mailto:preet98@yopmail.com"/>
+    <hyperlink ref="D23" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C23" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B23" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="AB23" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="AA23" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D29" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C29" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B29" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="S29" r:id="rId14" display="gita1@yopmail.com"/>
+    <hyperlink ref="D38" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C38" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B38" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D27" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C27" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B27" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D36" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C36" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B36" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D43" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C43" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B43" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="L43" r:id="rId15" display="luckysingh@yopmail.com"/>
+    <hyperlink ref="S43" r:id="rId15" display="luckysingh@yopmail.com"/>
+    <hyperlink ref="D44" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C44" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B44" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="L44" r:id="rId16" display="ramthakur@yopmail.com"/>
+    <hyperlink ref="D33" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C33" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B33" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D34" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C34" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B34" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="B35" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C35" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D35" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="B37" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C37" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D37" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="B39" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C39" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D39" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="B40" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D40" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C40" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Commit some code changes for some test cases
Commit some code changes for some test cases including mobile test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="301">
   <si>
     <t>TestData</t>
   </si>
@@ -1013,7 +1013,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="28">
+  <fonts count="29">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1061,6 +1061,12 @@
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="15"/>
+      <color rgb="FF040C28"/>
+      <name val="Arial"/>
+      <charset val="134"/>
     </font>
     <font>
       <sz val="11"/>
@@ -1570,13 +1576,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -1585,115 +1588,118 @@
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1714,9 +1720,6 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1728,13 +1731,14 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3545,10 +3549,10 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:AD46"/>
+  <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1:AD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
@@ -3578,7 +3582,7 @@
     <col min="28" max="28" width="24.7272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29">
+    <row r="1" ht="19" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3609,63 +3613,65 @@
       <c r="J1" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="L1" t="s">
+      <c r="L1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="M1" t="s">
+      <c r="M1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="N1" t="s">
+      <c r="N1" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="O1" t="s">
+      <c r="O1" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="P1" t="s">
+      <c r="P1" s="2" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="Q1" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="R1" t="s">
+      <c r="R1" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="S1" t="s">
+      <c r="S1" s="2" t="s">
         <v>114</v>
       </c>
-      <c r="T1" t="s">
+      <c r="T1" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="U1" t="s">
+      <c r="U1" s="2" t="s">
         <v>116</v>
       </c>
-      <c r="V1" t="s">
+      <c r="V1" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="W1" t="s">
+      <c r="W1" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="X1" t="s">
+      <c r="X1" s="2" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Y1" s="2" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="Z1" s="2" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AA1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AB1" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AC1" s="2" t="s">
         <v>17</v>
       </c>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="19"/>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" t="s">
@@ -4278,7 +4284,7 @@
       <c r="T8" t="s">
         <v>126</v>
       </c>
-      <c r="U8" s="15" t="s">
+      <c r="U8" s="14" t="s">
         <v>137</v>
       </c>
       <c r="V8" t="s">
@@ -4322,6 +4328,9 @@
       <c r="D9" t="s">
         <v>139</v>
       </c>
+      <c r="E9" t="s">
+        <v>63</v>
+      </c>
       <c r="F9" t="s">
         <v>63</v>
       </c>
@@ -4525,7 +4534,7 @@
       <c r="L11" t="s">
         <v>149</v>
       </c>
-      <c r="M11" s="5" t="s">
+      <c r="M11" s="3" t="s">
         <v>150</v>
       </c>
       <c r="N11" s="9" t="s">
@@ -4537,7 +4546,7 @@
       <c r="P11" s="9" t="s">
         <v>151</v>
       </c>
-      <c r="Q11" s="16" t="s">
+      <c r="Q11" s="15" t="s">
         <v>152</v>
       </c>
       <c r="R11" t="s">
@@ -4580,7 +4589,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="12" spans="1:18">
+    <row r="12" spans="1:30">
       <c r="A12" t="s">
         <v>53</v>
       </c>
@@ -4633,6 +4642,42 @@
         <v>63</v>
       </c>
       <c r="R12" t="s">
+        <v>63</v>
+      </c>
+      <c r="S12" t="s">
+        <v>63</v>
+      </c>
+      <c r="T12" t="s">
+        <v>63</v>
+      </c>
+      <c r="U12" t="s">
+        <v>63</v>
+      </c>
+      <c r="V12" t="s">
+        <v>63</v>
+      </c>
+      <c r="W12" t="s">
+        <v>63</v>
+      </c>
+      <c r="X12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC12" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD12" t="s">
         <v>63</v>
       </c>
     </row>
@@ -4759,7 +4804,7 @@
       <c r="J14" t="s">
         <v>63</v>
       </c>
-      <c r="K14" s="12" t="s">
+      <c r="K14" s="8" t="s">
         <v>159</v>
       </c>
       <c r="L14" t="s">
@@ -4820,7 +4865,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="15" spans="1:11">
+    <row r="15" spans="1:30">
       <c r="A15" t="s">
         <v>57</v>
       </c>
@@ -4854,8 +4899,65 @@
       <c r="K15" t="s">
         <v>162</v>
       </c>
-    </row>
-    <row r="16" spans="1:10">
+      <c r="L15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC15" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD15" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30">
       <c r="A16" t="s">
         <v>58</v>
       </c>
@@ -4868,6 +4970,9 @@
       <c r="D16" t="s">
         <v>88</v>
       </c>
+      <c r="E16" t="s">
+        <v>63</v>
+      </c>
       <c r="F16" t="s">
         <v>63</v>
       </c>
@@ -4883,8 +4988,68 @@
       <c r="J16" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="17" spans="1:20">
+      <c r="K16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC16" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD16" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30">
       <c r="A17" t="s">
         <v>59</v>
       </c>
@@ -4924,7 +5089,7 @@
       <c r="M17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N17" s="13" t="s">
+      <c r="N17" s="12" t="s">
         <v>165</v>
       </c>
       <c r="O17" s="7" t="s">
@@ -4933,7 +5098,7 @@
       <c r="P17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q17" s="17" t="s">
+      <c r="Q17" s="16" t="s">
         <v>166</v>
       </c>
       <c r="R17" s="7" t="s">
@@ -4945,8 +5110,38 @@
       <c r="T17" s="4" t="s">
         <v>168</v>
       </c>
-    </row>
-    <row r="18" spans="1:12">
+      <c r="U17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC17" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD17" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="18" spans="1:30">
       <c r="A18" t="s">
         <v>60</v>
       </c>
@@ -4983,8 +5178,62 @@
       <c r="L18" s="7" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="19" spans="1:11">
+      <c r="M18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC18" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD18" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:30">
       <c r="A19" s="7" t="s">
         <v>61</v>
       </c>
@@ -5018,8 +5267,65 @@
       <c r="K19" s="6" t="s">
         <v>172</v>
       </c>
-    </row>
-    <row r="20" spans="1:29">
+      <c r="L19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC19" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD19" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:30">
       <c r="A20" t="s">
         <v>173</v>
       </c>
@@ -5059,16 +5365,16 @@
       <c r="M20" t="s">
         <v>175</v>
       </c>
-      <c r="N20" s="14" t="s">
+      <c r="N20" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O20" t="s">
         <v>131</v>
       </c>
-      <c r="P20" s="14" t="s">
+      <c r="P20" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="Q20" s="16" t="s">
+      <c r="Q20" s="15" t="s">
         <v>178</v>
       </c>
       <c r="R20" t="s">
@@ -5107,8 +5413,11 @@
       <c r="AC20" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="21" spans="1:29">
+      <c r="AD20" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="21" spans="1:30">
       <c r="A21" s="8" t="s">
         <v>180</v>
       </c>
@@ -5148,16 +5457,16 @@
       <c r="M21" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="N21" s="14" t="s">
+      <c r="N21" s="13" t="s">
         <v>186</v>
       </c>
       <c r="O21" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="P21" s="14" t="s">
+      <c r="P21" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="Q21" s="16" t="s">
+      <c r="Q21" s="15" t="s">
         <v>133</v>
       </c>
       <c r="R21" s="8" t="s">
@@ -5196,8 +5505,11 @@
       <c r="AC21" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="22" spans="1:11">
+      <c r="AD21" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:30">
       <c r="A22" s="7" t="s">
         <v>75</v>
       </c>
@@ -5231,8 +5543,65 @@
       <c r="K22" s="6" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="23" spans="1:11">
+      <c r="L22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC22" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD22" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="23" spans="1:30">
       <c r="A23" s="7" t="s">
         <v>70</v>
       </c>
@@ -5266,8 +5635,65 @@
       <c r="K23" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="24" spans="1:11">
+      <c r="L23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC23" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD23" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="24" spans="1:30">
       <c r="A24" s="7" t="s">
         <v>62</v>
       </c>
@@ -5301,8 +5727,65 @@
       <c r="K24" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="25" spans="1:29">
+      <c r="L24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC24" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD24" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="25" spans="1:30">
       <c r="A25" t="s">
         <v>67</v>
       </c>
@@ -5342,16 +5825,16 @@
       <c r="M25" t="s">
         <v>175</v>
       </c>
-      <c r="N25" s="14" t="s">
+      <c r="N25" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O25" t="s">
         <v>131</v>
       </c>
-      <c r="P25" s="14" t="s">
+      <c r="P25" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="Q25" s="16" t="s">
+      <c r="Q25" s="15" t="s">
         <v>178</v>
       </c>
       <c r="R25" t="s">
@@ -5390,8 +5873,11 @@
       <c r="AC25" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="26" spans="1:9">
+      <c r="AD25" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="26" spans="1:30">
       <c r="A26" s="7" t="s">
         <v>194</v>
       </c>
@@ -5413,11 +5899,77 @@
       <c r="G26" s="7" t="s">
         <v>63</v>
       </c>
+      <c r="H26" s="7" t="s">
+        <v>63</v>
+      </c>
       <c r="I26" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="27" spans="1:26">
+      <c r="J26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="O26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="P26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="R26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="S26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="T26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="U26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC26" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD26" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="27" spans="1:30">
       <c r="A27" s="7" t="s">
         <v>197</v>
       </c>
@@ -5457,7 +6009,7 @@
       <c r="M27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N27" s="13">
+      <c r="N27" s="12">
         <v>500018</v>
       </c>
       <c r="O27" s="7" t="s">
@@ -5466,7 +6018,7 @@
       <c r="P27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q27" s="17" t="s">
+      <c r="Q27" s="16" t="s">
         <v>199</v>
       </c>
       <c r="R27" s="7" t="s">
@@ -5478,13 +6030,38 @@
       <c r="T27" s="6" t="s">
         <v>200</v>
       </c>
-      <c r="V27" s="10"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="10"/>
-      <c r="Y27" s="10"/>
-      <c r="Z27" s="10"/>
-    </row>
-    <row r="28" spans="1:20">
+      <c r="U27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC27" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD27" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="28" spans="1:30">
       <c r="A28" s="7" t="s">
         <v>201</v>
       </c>
@@ -5500,7 +6077,19 @@
       <c r="E28" s="6" t="s">
         <v>202</v>
       </c>
+      <c r="F28" t="s">
+        <v>63</v>
+      </c>
+      <c r="G28" t="s">
+        <v>63</v>
+      </c>
+      <c r="H28" t="s">
+        <v>63</v>
+      </c>
       <c r="I28" t="s">
+        <v>63</v>
+      </c>
+      <c r="J28" t="s">
         <v>63</v>
       </c>
       <c r="K28" s="6" t="s">
@@ -5512,7 +6101,7 @@
       <c r="M28" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N28" s="13" t="s">
+      <c r="N28" s="12" t="s">
         <v>165</v>
       </c>
       <c r="O28" s="7" t="s">
@@ -5521,7 +6110,7 @@
       <c r="P28" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q28" s="17" t="s">
+      <c r="Q28" s="16" t="s">
         <v>199</v>
       </c>
       <c r="R28" s="7" t="s">
@@ -5533,8 +6122,38 @@
       <c r="T28" s="4" t="s">
         <v>204</v>
       </c>
-    </row>
-    <row r="29" spans="1:29">
+      <c r="U28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="V28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="W28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="X28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC28" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD28" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="29" spans="1:30">
       <c r="A29" t="s">
         <v>205</v>
       </c>
@@ -5580,10 +6199,10 @@
       <c r="O29" t="s">
         <v>131</v>
       </c>
-      <c r="P29" s="14" t="s">
+      <c r="P29" s="13" t="s">
         <v>177</v>
       </c>
-      <c r="Q29" s="16" t="s">
+      <c r="Q29" s="15" t="s">
         <v>178</v>
       </c>
       <c r="R29" t="s">
@@ -5601,16 +6220,16 @@
       <c r="V29" s="10" t="s">
         <v>209</v>
       </c>
-      <c r="W29" s="17" t="s">
+      <c r="W29" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="X29" s="17" t="s">
+      <c r="X29" s="16" t="s">
         <v>211</v>
       </c>
-      <c r="Y29" s="17" t="s">
+      <c r="Y29" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="Z29" s="17" t="s">
+      <c r="Z29" s="16" t="s">
         <v>212</v>
       </c>
       <c r="AA29" t="s">
@@ -5622,8 +6241,11 @@
       <c r="AC29" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="30" spans="1:11">
+      <c r="AD29" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="30" spans="1:30">
       <c r="A30" s="7" t="s">
         <v>213</v>
       </c>
@@ -5642,14 +6264,80 @@
       <c r="F30" s="6" t="s">
         <v>215</v>
       </c>
+      <c r="G30" t="s">
+        <v>63</v>
+      </c>
+      <c r="H30" t="s">
+        <v>63</v>
+      </c>
       <c r="I30" t="s">
+        <v>63</v>
+      </c>
+      <c r="J30" t="s">
         <v>63</v>
       </c>
       <c r="K30" s="6" t="s">
         <v>215</v>
       </c>
-    </row>
-    <row r="31" spans="1:29">
+      <c r="L30" t="s">
+        <v>63</v>
+      </c>
+      <c r="M30" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" t="s">
+        <v>63</v>
+      </c>
+      <c r="P30" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q30" t="s">
+        <v>63</v>
+      </c>
+      <c r="R30" t="s">
+        <v>63</v>
+      </c>
+      <c r="S30" t="s">
+        <v>63</v>
+      </c>
+      <c r="T30" t="s">
+        <v>63</v>
+      </c>
+      <c r="U30" t="s">
+        <v>63</v>
+      </c>
+      <c r="V30" t="s">
+        <v>63</v>
+      </c>
+      <c r="W30" t="s">
+        <v>63</v>
+      </c>
+      <c r="X30" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>63</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC30" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD30" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="31" spans="1:30">
       <c r="A31" t="s">
         <v>216</v>
       </c>
@@ -5689,7 +6377,7 @@
       <c r="M31" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="14" t="s">
+      <c r="N31" s="13" t="s">
         <v>186</v>
       </c>
       <c r="O31" t="s">
@@ -5698,7 +6386,7 @@
       <c r="P31" t="s">
         <v>63</v>
       </c>
-      <c r="Q31" s="16" t="s">
+      <c r="Q31" s="15" t="s">
         <v>219</v>
       </c>
       <c r="R31" t="s">
@@ -5707,7 +6395,7 @@
       <c r="S31" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="T31" s="18" t="s">
+      <c r="T31" s="17" t="s">
         <v>220</v>
       </c>
       <c r="U31" t="s">
@@ -5716,16 +6404,16 @@
       <c r="V31" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W31" s="17" t="s">
+      <c r="W31" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="X31" s="17" t="s">
+      <c r="X31" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="Y31" s="17" t="s">
+      <c r="Y31" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="Z31" s="17" t="s">
+      <c r="Z31" s="16" t="s">
         <v>224</v>
       </c>
       <c r="AA31" t="s">
@@ -5737,8 +6425,11 @@
       <c r="AC31" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="32" spans="1:26">
+      <c r="AD31" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="32" spans="1:30">
       <c r="A32" s="7" t="s">
         <v>225</v>
       </c>
@@ -5817,8 +6508,20 @@
       <c r="Z32" s="10" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="33" spans="1:26">
+      <c r="AA32" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB32" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC32" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD32" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="33" spans="1:30">
       <c r="A33" s="7" t="s">
         <v>230</v>
       </c>
@@ -5858,7 +6561,7 @@
       <c r="M33" t="s">
         <v>63</v>
       </c>
-      <c r="N33" s="13" t="s">
+      <c r="N33" s="12" t="s">
         <v>233</v>
       </c>
       <c r="O33" s="7" t="s">
@@ -5867,7 +6570,7 @@
       <c r="P33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q33" s="17" t="s">
+      <c r="Q33" s="16" t="s">
         <v>199</v>
       </c>
       <c r="R33" s="7" t="s">
@@ -5897,8 +6600,20 @@
       <c r="Z33" s="10" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="34" spans="1:26">
+      <c r="AA33" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB33" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD33" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="34" spans="1:30">
       <c r="A34" s="7" t="s">
         <v>237</v>
       </c>
@@ -5962,23 +6677,35 @@
       <c r="U34" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V34" s="17" t="s">
+      <c r="V34" s="16" t="s">
         <v>221</v>
       </c>
-      <c r="W34" s="17" t="s">
+      <c r="W34" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="X34" s="17" t="s">
+      <c r="X34" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="Y34" s="17" t="s">
+      <c r="Y34" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="Z34" s="17" t="s">
+      <c r="Z34" s="16" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="35" spans="1:26">
+      <c r="AA34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD34" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="35" spans="1:30">
       <c r="A35" t="s">
         <v>241</v>
       </c>
@@ -6045,20 +6772,32 @@
       <c r="V35" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="W35" s="17" t="s">
+      <c r="W35" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="X35" s="17" t="s">
+      <c r="X35" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="Y35" s="17" t="s">
+      <c r="Y35" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="Z35" s="17" t="s">
+      <c r="Z35" s="16" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="36" spans="1:26">
+      <c r="AA35" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB35" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD35" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="36" spans="1:30">
       <c r="A36" t="s">
         <v>247</v>
       </c>
@@ -6125,20 +6864,32 @@
       <c r="V36" s="10" t="s">
         <v>250</v>
       </c>
-      <c r="W36" s="17" t="s">
+      <c r="W36" s="16" t="s">
         <v>251</v>
       </c>
-      <c r="X36" s="17" t="s">
+      <c r="X36" s="16" t="s">
         <v>252</v>
       </c>
-      <c r="Y36" s="17" t="s">
+      <c r="Y36" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="Z36" s="17" t="s">
+      <c r="Z36" s="16" t="s">
         <v>222</v>
       </c>
-    </row>
-    <row r="37" spans="1:26">
+      <c r="AA36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD36" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="37" spans="1:30">
       <c r="A37" s="7" t="s">
         <v>253</v>
       </c>
@@ -6178,7 +6929,7 @@
       <c r="M37" t="s">
         <v>63</v>
       </c>
-      <c r="N37" s="13" t="s">
+      <c r="N37" s="12" t="s">
         <v>256</v>
       </c>
       <c r="O37" s="7" t="s">
@@ -6196,7 +6947,7 @@
       <c r="S37" t="s">
         <v>167</v>
       </c>
-      <c r="T37" s="19" t="s">
+      <c r="T37" s="18" t="s">
         <v>257</v>
       </c>
       <c r="U37" t="s">
@@ -6205,20 +6956,32 @@
       <c r="V37" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W37" s="17" t="s">
+      <c r="W37" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="X37" s="17" t="s">
+      <c r="X37" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="Y37" s="17" t="s">
+      <c r="Y37" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="Z37" s="17" t="s">
+      <c r="Z37" s="16" t="s">
         <v>258</v>
       </c>
-    </row>
-    <row r="38" spans="1:29">
+      <c r="AA37" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB37" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD37" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="38" spans="1:30">
       <c r="A38" t="s">
         <v>259</v>
       </c>
@@ -6258,16 +7021,16 @@
       <c r="M38" t="s">
         <v>262</v>
       </c>
-      <c r="N38" s="14" t="s">
+      <c r="N38" s="13" t="s">
         <v>256</v>
       </c>
       <c r="O38" t="s">
         <v>131</v>
       </c>
-      <c r="P38" s="14" t="s">
+      <c r="P38" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="Q38" s="16" t="s">
+      <c r="Q38" s="15" t="s">
         <v>243</v>
       </c>
       <c r="R38" t="s">
@@ -6285,16 +7048,16 @@
       <c r="V38" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W38" s="17" t="s">
+      <c r="W38" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="X38" s="17" t="s">
+      <c r="X38" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="Y38" s="17" t="s">
+      <c r="Y38" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="Z38" s="17" t="s">
+      <c r="Z38" s="16" t="s">
         <v>224</v>
       </c>
       <c r="AA38" t="s">
@@ -6306,8 +7069,11 @@
       <c r="AC38" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="39" spans="1:26">
+      <c r="AD38" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="39" spans="1:30">
       <c r="A39" s="7" t="s">
         <v>264</v>
       </c>
@@ -6347,7 +7113,7 @@
       <c r="M39" t="s">
         <v>63</v>
       </c>
-      <c r="N39" s="13" t="s">
+      <c r="N39" s="12" t="s">
         <v>256</v>
       </c>
       <c r="O39" s="7" t="s">
@@ -6356,7 +7122,7 @@
       <c r="P39" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q39" s="17" t="s">
+      <c r="Q39" s="16" t="s">
         <v>243</v>
       </c>
       <c r="R39" t="s">
@@ -6374,10 +7140,10 @@
       <c r="V39" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W39" s="17" t="s">
+      <c r="W39" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="X39" s="17" t="s">
+      <c r="X39" s="16" t="s">
         <v>222</v>
       </c>
       <c r="Y39" s="10" t="s">
@@ -6386,8 +7152,20 @@
       <c r="Z39" s="10" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="40" spans="1:29">
+      <c r="AA39" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB39" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD39" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="40" spans="1:30">
       <c r="A40" t="s">
         <v>268</v>
       </c>
@@ -6427,7 +7205,7 @@
       <c r="M40" t="s">
         <v>63</v>
       </c>
-      <c r="N40" s="14" t="s">
+      <c r="N40" s="13" t="s">
         <v>256</v>
       </c>
       <c r="O40" t="s">
@@ -6436,7 +7214,7 @@
       <c r="P40" t="s">
         <v>63</v>
       </c>
-      <c r="Q40" s="16" t="s">
+      <c r="Q40" s="15" t="s">
         <v>133</v>
       </c>
       <c r="R40" t="s">
@@ -6454,16 +7232,16 @@
       <c r="V40" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W40" s="17" t="s">
+      <c r="W40" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="X40" s="17" t="s">
+      <c r="X40" s="16" t="s">
         <v>236</v>
       </c>
-      <c r="Y40" s="17" t="s">
+      <c r="Y40" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="Z40" s="17" t="s">
+      <c r="Z40" s="16" t="s">
         <v>224</v>
       </c>
       <c r="AA40" t="s">
@@ -6475,8 +7253,11 @@
       <c r="AC40" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="41" spans="1:26">
+      <c r="AD40" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="41" spans="1:30">
       <c r="A41" s="7" t="s">
         <v>271</v>
       </c>
@@ -6516,7 +7297,7 @@
       <c r="M41" t="s">
         <v>63</v>
       </c>
-      <c r="N41" s="13" t="s">
+      <c r="N41" s="12" t="s">
         <v>186</v>
       </c>
       <c r="O41" s="7" t="s">
@@ -6525,7 +7306,7 @@
       <c r="P41" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q41" s="17" t="s">
+      <c r="Q41" s="16" t="s">
         <v>274</v>
       </c>
       <c r="R41" t="s">
@@ -6555,8 +7336,20 @@
       <c r="Z41" s="10" t="s">
         <v>223</v>
       </c>
-    </row>
-    <row r="42" spans="1:26">
+      <c r="AA41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC41" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD41" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="42" spans="1:30">
       <c r="A42" s="7" t="s">
         <v>278</v>
       </c>
@@ -6596,7 +7389,7 @@
       <c r="M42" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N42" s="13" t="s">
+      <c r="N42" s="12" t="s">
         <v>281</v>
       </c>
       <c r="O42" s="7" t="s">
@@ -6605,7 +7398,7 @@
       <c r="P42" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q42" s="17" t="s">
+      <c r="Q42" s="16" t="s">
         <v>199</v>
       </c>
       <c r="R42" s="7" t="s">
@@ -6620,23 +7413,35 @@
       <c r="U42" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="V42" s="17" t="s">
+      <c r="V42" s="16" t="s">
         <v>244</v>
       </c>
-      <c r="W42" s="17" t="s">
+      <c r="W42" s="16" t="s">
         <v>245</v>
       </c>
-      <c r="X42" s="17" t="s">
+      <c r="X42" s="16" t="s">
         <v>246</v>
       </c>
-      <c r="Y42" s="17" t="s">
+      <c r="Y42" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="Z42" s="17" t="s">
+      <c r="Z42" s="16" t="s">
         <v>240</v>
       </c>
-    </row>
-    <row r="43" spans="1:26">
+      <c r="AA42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC42" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD42" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="43" spans="1:30">
       <c r="A43" s="7" t="s">
         <v>283</v>
       </c>
@@ -6676,7 +7481,7 @@
       <c r="M43" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N43" s="13" t="s">
+      <c r="N43" s="12" t="s">
         <v>186</v>
       </c>
       <c r="O43" s="7" t="s">
@@ -6685,7 +7490,7 @@
       <c r="P43" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q43" s="17" t="s">
+      <c r="Q43" s="16" t="s">
         <v>286</v>
       </c>
       <c r="R43" s="7" t="s">
@@ -6703,20 +7508,32 @@
       <c r="V43" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W43" s="17" t="s">
+      <c r="W43" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="X43" s="17" t="s">
+      <c r="X43" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="Y43" s="17" t="s">
+      <c r="Y43" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="Z43" s="17" t="s">
+      <c r="Z43" s="16" t="s">
         <v>229</v>
       </c>
-    </row>
-    <row r="44" spans="1:26">
+      <c r="AA43" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB43" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC43" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD43" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="44" spans="1:30">
       <c r="A44" s="7" t="s">
         <v>288</v>
       </c>
@@ -6756,7 +7573,7 @@
       <c r="M44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N44" s="13" t="s">
+      <c r="N44" s="12" t="s">
         <v>176</v>
       </c>
       <c r="O44" s="7" t="s">
@@ -6765,7 +7582,7 @@
       <c r="P44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q44" s="17" t="s">
+      <c r="Q44" s="16" t="s">
         <v>133</v>
       </c>
       <c r="R44" s="7" t="s">
@@ -6774,7 +7591,7 @@
       <c r="S44" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="T44" s="19" t="s">
+      <c r="T44" s="18" t="s">
         <v>257</v>
       </c>
       <c r="U44" s="7" t="s">
@@ -6783,20 +7600,32 @@
       <c r="V44" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W44" s="17" t="s">
+      <c r="W44" s="16" t="s">
         <v>235</v>
       </c>
-      <c r="X44" s="17" t="s">
+      <c r="X44" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="Y44" s="17" t="s">
+      <c r="Y44" s="16" t="s">
         <v>240</v>
       </c>
-      <c r="Z44" s="17" t="s">
+      <c r="Z44" s="16" t="s">
         <v>224</v>
       </c>
-    </row>
-    <row r="45" spans="1:29">
+      <c r="AA44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AB44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AC44" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD44" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:30">
       <c r="A45" t="s">
         <v>290</v>
       </c>
@@ -6836,16 +7665,16 @@
       <c r="M45" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="N45" s="14" t="s">
+      <c r="N45" s="13" t="s">
         <v>186</v>
       </c>
       <c r="O45" t="s">
         <v>131</v>
       </c>
-      <c r="P45" s="14" t="s">
+      <c r="P45" s="13" t="s">
         <v>263</v>
       </c>
-      <c r="Q45" s="16" t="s">
+      <c r="Q45" s="15" t="s">
         <v>294</v>
       </c>
       <c r="R45" t="s">
@@ -6863,16 +7692,16 @@
       <c r="V45" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W45" s="17" t="s">
+      <c r="W45" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="X45" s="17" t="s">
+      <c r="X45" s="16" t="s">
         <v>210</v>
       </c>
-      <c r="Y45" s="17" t="s">
+      <c r="Y45" s="16" t="s">
         <v>223</v>
       </c>
-      <c r="Z45" s="17" t="s">
+      <c r="Z45" s="16" t="s">
         <v>224</v>
       </c>
       <c r="AA45" t="s">
@@ -6884,8 +7713,11 @@
       <c r="AC45" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="46" spans="1:29">
+      <c r="AD45" s="7" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30">
       <c r="A46" t="s">
         <v>295</v>
       </c>
@@ -6925,16 +7757,16 @@
       <c r="M46" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="N46" s="14" t="s">
+      <c r="N46" s="13" t="s">
         <v>186</v>
       </c>
       <c r="O46" t="s">
         <v>131</v>
       </c>
-      <c r="P46" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q46" s="16" t="s">
+      <c r="P46" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q46" s="15" t="s">
         <v>300</v>
       </c>
       <c r="R46" t="s">
@@ -6952,16 +7784,16 @@
       <c r="V46" s="10" t="s">
         <v>221</v>
       </c>
-      <c r="W46" s="17" t="s">
+      <c r="W46" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="X46" s="17" t="s">
+      <c r="X46" s="16" t="s">
         <v>222</v>
       </c>
-      <c r="Y46" s="17" t="s">
+      <c r="Y46" s="16" t="s">
         <v>228</v>
       </c>
-      <c r="Z46" s="17" t="s">
+      <c r="Z46" s="16" t="s">
         <v>229</v>
       </c>
       <c r="AA46" t="s">
@@ -6971,6 +7803,9 @@
         <v>63</v>
       </c>
       <c r="AC46" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD46" s="7" t="s">
         <v>63</v>
       </c>
     </row>
@@ -7028,7 +7863,7 @@
     <hyperlink ref="D8" r:id="rId5" display="Kdeep@98"/>
     <hyperlink ref="B11" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="G11" r:id="rId9" display="dhanya@yopmail.com" tooltip="mailto:dhanya@yopmail.com"/>
-    <hyperlink ref="M11" r:id="rId10" display="shardha@yopmail.com"/>
+    <hyperlink ref="M11" r:id="rId10" display="shardha@yopmail.com" tooltip="mailto:shardha@yopmail.com"/>
     <hyperlink ref="B12" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="B26" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D26" r:id="rId2" display="Sah@6057"/>

</xml_diff>

<commit_message>
Committing code changes in few test cases
Committing code changes in few test cases
</commit_message>
<xml_diff>
--- a/src/test/resources/testData/TestData.xlsx
+++ b/src/test/resources/testData/TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="18350" windowHeight="6830" activeTab="2"/>
+    <workbookView windowWidth="18345" windowHeight="6810" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="ACS" sheetId="8" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="301">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1796" uniqueCount="303">
   <si>
     <t>TestData</t>
   </si>
@@ -567,7 +567,7 @@
     <t>Testdata23</t>
   </si>
   <si>
-    <t>Tx-Testing</t>
+    <t>Tx-Testing18161418</t>
   </si>
   <si>
     <t>rahul1234@yopmail.com</t>
@@ -669,6 +669,9 @@
     <t>TX_16</t>
   </si>
   <si>
+    <t>Tx-Testing</t>
+  </si>
+  <si>
     <t>Ask about activities that they do with others,PROMIS-29</t>
   </si>
   <si>
@@ -861,7 +864,7 @@
     <t>125055</t>
   </si>
   <si>
-    <t>Rahul98@yopmail.com</t>
+    <t>Karan98@yopmail.com</t>
   </si>
   <si>
     <t>5.5</t>
@@ -967,6 +970,9 @@
   </si>
   <si>
     <t>Tx-Testing10</t>
+  </si>
+  <si>
+    <t>Rahul98@yopmail.com</t>
   </si>
   <si>
     <t>Testdata49</t>
@@ -1013,7 +1019,7 @@
     <numFmt numFmtId="179" formatCode="_ &quot;₹&quot;* #,##0_ ;_ &quot;₹&quot;* \-#,##0_ ;_ &quot;₹&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="180" formatCode="0.00_);[Red]\(0.00\)"/>
   </numFmts>
-  <fonts count="29">
+  <fonts count="32">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1025,6 +1031,28 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF454A4A"/>
+      <name val="Arial"/>
       <charset val="134"/>
     </font>
     <font>
@@ -1576,134 +1604,134 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1715,30 +1743,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="180" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="6" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="6" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2004,27 +2035,27 @@
       <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90909090909091" defaultRowHeight="13.5" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="8.90476190476191" defaultRowHeight="13.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="13.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="49.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="1" max="1" width="13.5428571428571" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="49.4571428571429" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="26" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="11.0909090909091" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="11.0952380952381" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="19" customWidth="1" collapsed="1"/>
-    <col min="6" max="6" width="33.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="24.6363636363636" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="33.1809523809524" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="24.6380952380952" customWidth="1" collapsed="1"/>
     <col min="8" max="8" width="19" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="19.7272727272727" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="64.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="28.1818181818182" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="102.181818181818" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="19.9090909090909" customWidth="1" collapsed="1"/>
-    <col min="16" max="16" width="26.6363636363636" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="30.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="25.8181818181818" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="19.7238095238095" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="64.2761904761905" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="28.1809523809524" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="102.180952380952" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="19.9047619047619" customWidth="1" collapsed="1"/>
+    <col min="16" max="16" width="26.6380952380952" customWidth="1" collapsed="1"/>
+    <col min="17" max="17" width="30.5428571428571" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="25.8190476190476" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="14.5" spans="1:18">
+    <row r="1" ht="15" spans="1:18">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2080,7 +2111,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" ht="14.5" spans="1:11">
+    <row r="2" ht="15" spans="1:11">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -2115,7 +2146,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" ht="14.5" spans="1:12">
+    <row r="3" ht="15" spans="1:12">
       <c r="A3" t="s">
         <v>29</v>
       </c>
@@ -2149,11 +2180,11 @@
       <c r="K3" t="s">
         <v>28</v>
       </c>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="26" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="4" ht="14.5" spans="1:12">
+    <row r="4" ht="15" spans="1:12">
       <c r="A4" t="s">
         <v>31</v>
       </c>
@@ -2191,7 +2222,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="5" ht="14.5" spans="1:12">
+    <row r="5" ht="15" spans="1:12">
       <c r="A5" t="s">
         <v>34</v>
       </c>
@@ -2225,7 +2256,7 @@
       <c r="K5" t="s">
         <v>35</v>
       </c>
-      <c r="L5" s="23" t="s">
+      <c r="L5" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2263,11 +2294,11 @@
       <c r="K6" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="23" t="s">
+      <c r="L6" s="26" t="s">
         <v>38</v>
       </c>
       <c r="M6" s="5"/>
-      <c r="T6" s="23"/>
+      <c r="T6" s="26"/>
     </row>
     <row r="7" customHeight="1" spans="1:12">
       <c r="A7" t="s">
@@ -2335,7 +2366,7 @@
       <c r="I8" t="s">
         <v>44</v>
       </c>
-      <c r="J8" s="11" t="s">
+      <c r="J8" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K8" t="s">
@@ -2370,13 +2401,13 @@
       <c r="I9" t="s">
         <v>44</v>
       </c>
-      <c r="J9" s="11" t="s">
+      <c r="J9" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K9" t="s">
         <v>35</v>
       </c>
-      <c r="L9" s="23" t="s">
+      <c r="L9" s="26" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2408,7 +2439,7 @@
       <c r="I10" t="s">
         <v>44</v>
       </c>
-      <c r="J10" s="11" t="s">
+      <c r="J10" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K10" t="s">
@@ -2443,7 +2474,7 @@
       <c r="I11" t="s">
         <v>26</v>
       </c>
-      <c r="J11" s="11" t="s">
+      <c r="J11" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K11" t="s">
@@ -2481,13 +2512,13 @@
       <c r="I12" t="s">
         <v>26</v>
       </c>
-      <c r="J12" s="11" t="s">
+      <c r="J12" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K12" t="s">
         <v>35</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2519,13 +2550,13 @@
       <c r="I13" t="s">
         <v>26</v>
       </c>
-      <c r="J13" s="11" t="s">
+      <c r="J13" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K13" t="s">
         <v>35</v>
       </c>
-      <c r="L13" s="23" t="s">
+      <c r="L13" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2557,7 +2588,7 @@
       <c r="I14" t="s">
         <v>26</v>
       </c>
-      <c r="J14" s="11" t="s">
+      <c r="J14" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K14" t="s">
@@ -2636,7 +2667,7 @@
       <c r="K16" t="s">
         <v>35</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="L16" s="26" t="s">
         <v>30</v>
       </c>
     </row>
@@ -2712,7 +2743,7 @@
       <c r="K18" t="s">
         <v>35</v>
       </c>
-      <c r="L18" s="23" t="s">
+      <c r="L18" s="26" t="s">
         <v>36</v>
       </c>
     </row>
@@ -2750,7 +2781,7 @@
       <c r="K19" t="s">
         <v>35</v>
       </c>
-      <c r="L19" s="23" t="s">
+      <c r="L19" s="26" t="s">
         <v>38</v>
       </c>
     </row>
@@ -2820,7 +2851,7 @@
       <c r="I21" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="11" t="s">
+      <c r="J21" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K21" t="s">
@@ -2838,7 +2869,7 @@
       <c r="O21" t="s">
         <v>63</v>
       </c>
-      <c r="P21" s="11" t="s">
+      <c r="P21" s="14" t="s">
         <v>64</v>
       </c>
       <c r="Q21" s="3" t="s">
@@ -2876,7 +2907,7 @@
       <c r="I22" t="s">
         <v>44</v>
       </c>
-      <c r="J22" s="11" t="s">
+      <c r="J22" s="14" t="s">
         <v>45</v>
       </c>
       <c r="K22" t="s">
@@ -3085,19 +3116,19 @@
       <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="15" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="53.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="41.0909090909091" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="5" max="6" width="24.5454545454545" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="30.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="14.2727272727273" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="35.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="41.4545454545455" customWidth="1" collapsed="1"/>
-    <col min="11" max="11" width="27.8181818181818" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="16.4545454545455" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="53.4571428571429" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="41.0952380952381" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.8190476190476" customWidth="1" collapsed="1"/>
+    <col min="5" max="6" width="24.5428571428571" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="30.8190476190476" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="14.2761904761905" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="35.4571428571429" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="41.4571428571429" customWidth="1" collapsed="1"/>
+    <col min="11" max="11" width="27.8190476190476" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="16.4571428571429" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14">
@@ -3198,13 +3229,13 @@
       <c r="H3" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I3" s="21" t="s">
+      <c r="I3" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="J3" s="21" t="s">
+      <c r="J3" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="K3" s="21" t="s">
+      <c r="K3" s="24" t="s">
         <v>88</v>
       </c>
     </row>
@@ -3239,7 +3270,7 @@
       <c r="J4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="K4" s="20" t="s">
+      <c r="K4" s="23" t="s">
         <v>66</v>
       </c>
     </row>
@@ -3253,7 +3284,7 @@
       <c r="C5" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="23" t="s">
         <v>66</v>
       </c>
       <c r="E5" t="s">
@@ -3373,7 +3404,7 @@
       <c r="H8" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="I8" s="27" t="s">
         <v>101</v>
       </c>
     </row>
@@ -3551,38 +3582,38 @@
   <sheetPr/>
   <dimension ref="A1:AE46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="K1" sqref="K1:AD1"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37:Z37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultColWidth="8.72380952380952" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.4545454545455" customWidth="1"/>
-    <col min="2" max="2" width="52.8181818181818" customWidth="1"/>
-    <col min="3" max="3" width="38.9090909090909" customWidth="1"/>
-    <col min="4" max="4" width="18.2727272727273" customWidth="1"/>
-    <col min="5" max="5" width="23.4545454545455" customWidth="1"/>
-    <col min="6" max="6" width="17.6363636363636" customWidth="1"/>
-    <col min="7" max="7" width="41.1818181818182" customWidth="1"/>
-    <col min="8" max="8" width="22.3636363636364" customWidth="1"/>
-    <col min="9" max="10" width="24.8181818181818" customWidth="1"/>
+    <col min="1" max="1" width="16.4571428571429" customWidth="1"/>
+    <col min="2" max="2" width="52.8190476190476" customWidth="1"/>
+    <col min="3" max="3" width="38.9047619047619" customWidth="1"/>
+    <col min="4" max="4" width="18.2761904761905" customWidth="1"/>
+    <col min="5" max="5" width="23.4571428571429" customWidth="1"/>
+    <col min="6" max="6" width="17.6380952380952" customWidth="1"/>
+    <col min="7" max="7" width="41.1809523809524" customWidth="1"/>
+    <col min="8" max="8" width="22.3619047619048" customWidth="1"/>
+    <col min="9" max="10" width="24.8190476190476" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="15.3636363636364" customWidth="1"/>
-    <col min="13" max="13" width="26.6363636363636" customWidth="1"/>
-    <col min="14" max="14" width="15.3636363636364" customWidth="1"/>
-    <col min="15" max="15" width="13.7272727272727" customWidth="1"/>
-    <col min="17" max="17" width="17.4545454545455" customWidth="1"/>
-    <col min="19" max="19" width="26.3636363636364" customWidth="1"/>
-    <col min="20" max="20" width="23.5454545454545" customWidth="1"/>
-    <col min="21" max="21" width="18.7272727272727" customWidth="1"/>
-    <col min="22" max="22" width="16.4545454545455" customWidth="1"/>
-    <col min="23" max="23" width="13.0909090909091" customWidth="1"/>
-    <col min="24" max="24" width="13.5454545454545" customWidth="1"/>
-    <col min="25" max="25" width="13.9090909090909" customWidth="1"/>
-    <col min="28" max="28" width="24.7272727272727" customWidth="1"/>
+    <col min="12" max="12" width="15.3619047619048" customWidth="1"/>
+    <col min="13" max="13" width="26.6380952380952" customWidth="1"/>
+    <col min="14" max="14" width="15.3619047619048" customWidth="1"/>
+    <col min="15" max="15" width="13.7238095238095" customWidth="1"/>
+    <col min="17" max="17" width="17.4571428571429" customWidth="1"/>
+    <col min="19" max="19" width="26.3619047619048" customWidth="1"/>
+    <col min="20" max="20" width="23.5428571428571" customWidth="1"/>
+    <col min="21" max="21" width="18.7238095238095" customWidth="1"/>
+    <col min="22" max="22" width="16.4571428571429" customWidth="1"/>
+    <col min="23" max="23" width="13.0952380952381" customWidth="1"/>
+    <col min="24" max="24" width="13.5428571428571" customWidth="1"/>
+    <col min="25" max="25" width="13.9047619047619" customWidth="1"/>
+    <col min="28" max="28" width="24.7238095238095" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="19" spans="1:31">
+    <row r="1" ht="18.75" spans="1:31">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3671,7 +3702,7 @@
         <v>17</v>
       </c>
       <c r="AD1" s="2"/>
-      <c r="AE1" s="19"/>
+      <c r="AE1" s="22"/>
     </row>
     <row r="2" spans="1:30">
       <c r="A2" t="s">
@@ -3989,16 +4020,16 @@
       <c r="M5" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="N5" s="9" t="s">
+      <c r="N5" s="12" t="s">
         <v>130</v>
       </c>
       <c r="O5" t="s">
         <v>131</v>
       </c>
-      <c r="P5" s="9" t="s">
+      <c r="P5" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="13" t="s">
         <v>133</v>
       </c>
       <c r="R5" t="s">
@@ -4081,16 +4112,16 @@
       <c r="M6" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="N6" s="9" t="s">
+      <c r="N6" s="12" t="s">
         <v>130</v>
       </c>
       <c r="O6" t="s">
         <v>131</v>
       </c>
-      <c r="P6" s="9" t="s">
+      <c r="P6" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="13" t="s">
         <v>133</v>
       </c>
       <c r="R6" t="s">
@@ -4173,16 +4204,16 @@
       <c r="M7" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="N7" s="9" t="s">
+      <c r="N7" s="12" t="s">
         <v>130</v>
       </c>
       <c r="O7" t="s">
         <v>131</v>
       </c>
-      <c r="P7" s="9" t="s">
+      <c r="P7" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="13" t="s">
         <v>133</v>
       </c>
       <c r="R7" t="s">
@@ -4265,8 +4296,8 @@
       <c r="M8" t="s">
         <v>131</v>
       </c>
-      <c r="N8" s="9"/>
-      <c r="O8" s="10" t="s">
+      <c r="N8" s="12"/>
+      <c r="O8" s="13" t="s">
         <v>133</v>
       </c>
       <c r="P8" t="s">
@@ -4284,7 +4315,7 @@
       <c r="T8" t="s">
         <v>126</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="U8" s="17" t="s">
         <v>137</v>
       </c>
       <c r="V8" t="s">
@@ -4445,16 +4476,16 @@
       <c r="M10" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="N10" s="9" t="s">
+      <c r="N10" s="12" t="s">
         <v>130</v>
       </c>
       <c r="O10" t="s">
         <v>131</v>
       </c>
-      <c r="P10" s="9" t="s">
+      <c r="P10" s="12" t="s">
         <v>132</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="Q10" s="13" t="s">
         <v>133</v>
       </c>
       <c r="R10" t="s">
@@ -4522,7 +4553,7 @@
       <c r="H11" t="s">
         <v>95</v>
       </c>
-      <c r="I11" s="11" t="s">
+      <c r="I11" s="14" t="s">
         <v>92</v>
       </c>
       <c r="J11" t="s">
@@ -4537,16 +4568,16 @@
       <c r="M11" s="3" t="s">
         <v>150</v>
       </c>
-      <c r="N11" s="9" t="s">
+      <c r="N11" s="12" t="s">
         <v>132</v>
       </c>
       <c r="O11" t="s">
         <v>131</v>
       </c>
-      <c r="P11" s="9" t="s">
+      <c r="P11" s="12" t="s">
         <v>151</v>
       </c>
-      <c r="Q11" s="15" t="s">
+      <c r="Q11" s="18" t="s">
         <v>152</v>
       </c>
       <c r="R11" t="s">
@@ -4813,7 +4844,7 @@
       <c r="M14" t="s">
         <v>161</v>
       </c>
-      <c r="N14" s="9" t="s">
+      <c r="N14" s="12" t="s">
         <v>130</v>
       </c>
       <c r="O14" t="s">
@@ -5089,7 +5120,7 @@
       <c r="M17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N17" s="12" t="s">
+      <c r="N17" s="15" t="s">
         <v>165</v>
       </c>
       <c r="O17" s="7" t="s">
@@ -5098,7 +5129,7 @@
       <c r="P17" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q17" s="16" t="s">
+      <c r="Q17" s="19" t="s">
         <v>166</v>
       </c>
       <c r="R17" s="7" t="s">
@@ -5365,16 +5396,16 @@
       <c r="M20" t="s">
         <v>175</v>
       </c>
-      <c r="N20" s="13" t="s">
+      <c r="N20" s="16" t="s">
         <v>176</v>
       </c>
       <c r="O20" t="s">
         <v>131</v>
       </c>
-      <c r="P20" s="13" t="s">
+      <c r="P20" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Q20" s="15" t="s">
+      <c r="Q20" s="18" t="s">
         <v>178</v>
       </c>
       <c r="R20" t="s">
@@ -5457,16 +5488,16 @@
       <c r="M21" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="N21" s="13" t="s">
+      <c r="N21" s="16" t="s">
         <v>186</v>
       </c>
       <c r="O21" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="P21" s="13" t="s">
+      <c r="P21" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Q21" s="15" t="s">
+      <c r="Q21" s="18" t="s">
         <v>133</v>
       </c>
       <c r="R21" s="8" t="s">
@@ -5694,22 +5725,22 @@
       </c>
     </row>
     <row r="24" spans="1:30">
-      <c r="A24" s="7" t="s">
+      <c r="A24" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="D24" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="6" t="s">
+      <c r="E24" s="11" t="s">
         <v>192</v>
       </c>
-      <c r="F24" s="7" t="s">
+      <c r="F24" t="s">
         <v>63</v>
       </c>
       <c r="G24" t="s">
@@ -5799,7 +5830,7 @@
         <v>21</v>
       </c>
       <c r="E25" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="F25" t="s">
         <v>135</v>
@@ -5825,16 +5856,16 @@
       <c r="M25" t="s">
         <v>175</v>
       </c>
-      <c r="N25" s="13" t="s">
+      <c r="N25" s="16" t="s">
         <v>176</v>
       </c>
       <c r="O25" t="s">
         <v>131</v>
       </c>
-      <c r="P25" s="13" t="s">
+      <c r="P25" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Q25" s="15" t="s">
+      <c r="Q25" s="18" t="s">
         <v>178</v>
       </c>
       <c r="R25" t="s">
@@ -5865,7 +5896,7 @@
         <v>63</v>
       </c>
       <c r="AA25" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AB25" s="3" t="s">
         <v>20</v>
@@ -5879,7 +5910,7 @@
     </row>
     <row r="26" spans="1:30">
       <c r="A26" s="7" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B26" s="3" t="s">
         <v>19</v>
@@ -5891,10 +5922,10 @@
         <v>21</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="F26" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="G26" s="7" t="s">
         <v>63</v>
@@ -5971,7 +6002,7 @@
     </row>
     <row r="27" spans="1:30">
       <c r="A27" s="7" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>19</v>
@@ -5983,7 +6014,7 @@
         <v>21</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="F27" s="7" t="s">
         <v>63</v>
@@ -6009,7 +6040,7 @@
       <c r="M27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N27" s="12">
+      <c r="N27" s="15">
         <v>500018</v>
       </c>
       <c r="O27" s="7" t="s">
@@ -6018,8 +6049,8 @@
       <c r="P27" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q27" s="16" t="s">
-        <v>199</v>
+      <c r="Q27" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="R27" s="7" t="s">
         <v>63</v>
@@ -6028,7 +6059,7 @@
         <v>167</v>
       </c>
       <c r="T27" s="6" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="U27" s="7" t="s">
         <v>63</v>
@@ -6063,7 +6094,7 @@
     </row>
     <row r="28" spans="1:30">
       <c r="A28" s="7" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>19</v>
@@ -6075,7 +6106,7 @@
         <v>21</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="F28" t="s">
         <v>63</v>
@@ -6093,7 +6124,7 @@
         <v>63</v>
       </c>
       <c r="K28" s="6" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="L28" s="7" t="s">
         <v>63</v>
@@ -6101,7 +6132,7 @@
       <c r="M28" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N28" s="12" t="s">
+      <c r="N28" s="15" t="s">
         <v>165</v>
       </c>
       <c r="O28" s="7" t="s">
@@ -6110,8 +6141,8 @@
       <c r="P28" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q28" s="16" t="s">
-        <v>199</v>
+      <c r="Q28" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="R28" s="7" t="s">
         <v>63</v>
@@ -6120,7 +6151,7 @@
         <v>167</v>
       </c>
       <c r="T28" s="4" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="U28" s="7" t="s">
         <v>63</v>
@@ -6155,7 +6186,7 @@
     </row>
     <row r="29" spans="1:30">
       <c r="A29" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>19</v>
@@ -6167,7 +6198,7 @@
         <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="F29" t="s">
         <v>63</v>
@@ -6185,24 +6216,24 @@
         <v>63</v>
       </c>
       <c r="K29" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="L29" t="s">
         <v>128</v>
       </c>
       <c r="M29" t="s">
-        <v>208</v>
-      </c>
-      <c r="N29" s="10" t="s">
+        <v>209</v>
+      </c>
+      <c r="N29" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O29" t="s">
         <v>131</v>
       </c>
-      <c r="P29" s="13" t="s">
+      <c r="P29" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="Q29" s="15" t="s">
+      <c r="Q29" s="18" t="s">
         <v>178</v>
       </c>
       <c r="R29" t="s">
@@ -6217,23 +6248,23 @@
       <c r="U29" t="s">
         <v>63</v>
       </c>
-      <c r="V29" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="W29" s="16" t="s">
+      <c r="V29" s="13" t="s">
         <v>210</v>
       </c>
-      <c r="X29" s="16" t="s">
+      <c r="W29" s="19" t="s">
         <v>211</v>
       </c>
-      <c r="Y29" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z29" s="16" t="s">
+      <c r="X29" s="19" t="s">
         <v>212</v>
       </c>
+      <c r="Y29" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z29" s="19" t="s">
+        <v>213</v>
+      </c>
       <c r="AA29" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="AB29" t="s">
         <v>20</v>
@@ -6247,7 +6278,7 @@
     </row>
     <row r="30" spans="1:30">
       <c r="A30" s="7" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>19</v>
@@ -6259,10 +6290,10 @@
         <v>21</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="G30" t="s">
         <v>63</v>
@@ -6277,7 +6308,7 @@
         <v>63</v>
       </c>
       <c r="K30" s="6" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="L30" t="s">
         <v>63</v>
@@ -6339,7 +6370,7 @@
     </row>
     <row r="31" spans="1:30">
       <c r="A31" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>19</v>
@@ -6351,7 +6382,7 @@
         <v>21</v>
       </c>
       <c r="E31" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="F31" t="s">
         <v>63</v>
@@ -6369,7 +6400,7 @@
         <v>63</v>
       </c>
       <c r="K31" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="L31" t="s">
         <v>63</v>
@@ -6377,7 +6408,7 @@
       <c r="M31" t="s">
         <v>63</v>
       </c>
-      <c r="N31" s="13" t="s">
+      <c r="N31" s="16" t="s">
         <v>186</v>
       </c>
       <c r="O31" t="s">
@@ -6386,8 +6417,8 @@
       <c r="P31" t="s">
         <v>63</v>
       </c>
-      <c r="Q31" s="15" t="s">
-        <v>219</v>
+      <c r="Q31" s="18" t="s">
+        <v>220</v>
       </c>
       <c r="R31" t="s">
         <v>63</v>
@@ -6395,26 +6426,26 @@
       <c r="S31" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="T31" s="17" t="s">
-        <v>220</v>
+      <c r="T31" s="20" t="s">
+        <v>221</v>
       </c>
       <c r="U31" t="s">
         <v>63</v>
       </c>
-      <c r="V31" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W31" s="16" t="s">
+      <c r="V31" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="X31" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="Y31" s="16" t="s">
+      <c r="W31" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="Z31" s="16" t="s">
+      <c r="X31" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y31" s="19" t="s">
         <v>224</v>
+      </c>
+      <c r="Z31" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="AA31" t="s">
         <v>63</v>
@@ -6431,7 +6462,7 @@
     </row>
     <row r="32" spans="1:30">
       <c r="A32" s="7" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>19</v>
@@ -6443,7 +6474,7 @@
         <v>21</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="F32" t="s">
         <v>63</v>
@@ -6461,7 +6492,7 @@
         <v>63</v>
       </c>
       <c r="K32" s="6" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="L32" s="7" t="s">
         <v>63</v>
@@ -6493,20 +6524,20 @@
       <c r="U32" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V32" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W32" s="10" t="s">
+      <c r="V32" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="X32" s="10" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y32" s="10" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z32" s="10" t="s">
+      <c r="W32" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="X32" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y32" s="13" t="s">
         <v>229</v>
+      </c>
+      <c r="Z32" s="13" t="s">
+        <v>230</v>
       </c>
       <c r="AA32" t="s">
         <v>63</v>
@@ -6523,7 +6554,7 @@
     </row>
     <row r="33" spans="1:30">
       <c r="A33" s="7" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>19</v>
@@ -6535,7 +6566,7 @@
         <v>21</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="F33" t="s">
         <v>63</v>
@@ -6553,7 +6584,7 @@
         <v>63</v>
       </c>
       <c r="K33" s="6" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="L33" t="s">
         <v>63</v>
@@ -6561,8 +6592,8 @@
       <c r="M33" t="s">
         <v>63</v>
       </c>
-      <c r="N33" s="12" t="s">
-        <v>233</v>
+      <c r="N33" s="15" t="s">
+        <v>234</v>
       </c>
       <c r="O33" s="7" t="s">
         <v>63</v>
@@ -6570,8 +6601,8 @@
       <c r="P33" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q33" s="16" t="s">
-        <v>199</v>
+      <c r="Q33" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="R33" s="7" t="s">
         <v>63</v>
@@ -6580,25 +6611,25 @@
         <v>167</v>
       </c>
       <c r="T33" s="4" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="U33" t="s">
         <v>63</v>
       </c>
-      <c r="V33" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W33" s="10" t="s">
-        <v>235</v>
-      </c>
-      <c r="X33" s="10" t="s">
+      <c r="V33" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="W33" s="13" t="s">
         <v>236</v>
       </c>
-      <c r="Y33" s="10" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z33" s="10" t="s">
+      <c r="X33" s="13" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y33" s="13" t="s">
         <v>224</v>
+      </c>
+      <c r="Z33" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="AA33" t="s">
         <v>63</v>
@@ -6615,7 +6646,7 @@
     </row>
     <row r="34" spans="1:30">
       <c r="A34" s="7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="B34" s="3" t="s">
         <v>19</v>
@@ -6627,7 +6658,7 @@
         <v>21</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="F34" t="s">
         <v>63</v>
@@ -6645,7 +6676,7 @@
         <v>63</v>
       </c>
       <c r="K34" s="6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="L34" s="7" t="s">
         <v>63</v>
@@ -6677,20 +6708,20 @@
       <c r="U34" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V34" s="16" t="s">
-        <v>221</v>
-      </c>
-      <c r="W34" s="16" t="s">
+      <c r="V34" s="19" t="s">
         <v>222</v>
       </c>
-      <c r="X34" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y34" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="Z34" s="16" t="s">
-        <v>224</v>
+      <c r="W34" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="X34" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y34" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z34" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="AA34" t="s">
         <v>63</v>
@@ -6707,7 +6738,7 @@
     </row>
     <row r="35" spans="1:30">
       <c r="A35" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B35" s="3" t="s">
         <v>19</v>
@@ -6719,7 +6750,7 @@
         <v>21</v>
       </c>
       <c r="E35" t="s">
-        <v>174</v>
+        <v>193</v>
       </c>
       <c r="F35" t="s">
         <v>63</v>
@@ -6737,7 +6768,7 @@
         <v>63</v>
       </c>
       <c r="K35" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L35" t="s">
         <v>63</v>
@@ -6745,7 +6776,7 @@
       <c r="M35" t="s">
         <v>63</v>
       </c>
-      <c r="N35" s="10" t="s">
+      <c r="N35" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O35" t="s">
@@ -6754,8 +6785,8 @@
       <c r="P35" t="s">
         <v>63</v>
       </c>
-      <c r="Q35" s="10" t="s">
-        <v>243</v>
+      <c r="Q35" s="13" t="s">
+        <v>244</v>
       </c>
       <c r="R35" t="s">
         <v>63</v>
@@ -6769,20 +6800,20 @@
       <c r="U35" t="s">
         <v>63</v>
       </c>
-      <c r="V35" s="10" t="s">
-        <v>244</v>
-      </c>
-      <c r="W35" s="16" t="s">
+      <c r="V35" s="13" t="s">
         <v>245</v>
       </c>
-      <c r="X35" s="16" t="s">
+      <c r="W35" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="Y35" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z35" s="16" t="s">
-        <v>240</v>
+      <c r="X35" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y35" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z35" s="19" t="s">
+        <v>241</v>
       </c>
       <c r="AA35" t="s">
         <v>63</v>
@@ -6799,7 +6830,7 @@
     </row>
     <row r="36" spans="1:30">
       <c r="A36" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>19</v>
@@ -6811,7 +6842,7 @@
         <v>21</v>
       </c>
       <c r="E36" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="F36" t="s">
         <v>63</v>
@@ -6829,7 +6860,7 @@
         <v>63</v>
       </c>
       <c r="K36" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L36" t="s">
         <v>63</v>
@@ -6837,7 +6868,7 @@
       <c r="M36" t="s">
         <v>63</v>
       </c>
-      <c r="N36" s="10" t="s">
+      <c r="N36" s="13" t="s">
         <v>176</v>
       </c>
       <c r="O36" t="s">
@@ -6846,7 +6877,7 @@
       <c r="P36" t="s">
         <v>63</v>
       </c>
-      <c r="Q36" s="10" t="s">
+      <c r="Q36" s="13" t="s">
         <v>178</v>
       </c>
       <c r="R36" t="s">
@@ -6861,20 +6892,20 @@
       <c r="U36" t="s">
         <v>63</v>
       </c>
-      <c r="V36" s="10" t="s">
-        <v>250</v>
-      </c>
-      <c r="W36" s="16" t="s">
+      <c r="V36" s="13" t="s">
         <v>251</v>
       </c>
-      <c r="X36" s="16" t="s">
+      <c r="W36" s="19" t="s">
         <v>252</v>
       </c>
-      <c r="Y36" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z36" s="16" t="s">
-        <v>222</v>
+      <c r="X36" s="19" t="s">
+        <v>253</v>
+      </c>
+      <c r="Y36" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z36" s="19" t="s">
+        <v>223</v>
       </c>
       <c r="AA36" t="s">
         <v>63</v>
@@ -6890,22 +6921,22 @@
       </c>
     </row>
     <row r="37" spans="1:30">
-      <c r="A37" s="7" t="s">
-        <v>253</v>
-      </c>
-      <c r="B37" s="3" t="s">
+      <c r="A37" t="s">
+        <v>254</v>
+      </c>
+      <c r="B37" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="4" t="s">
+      <c r="D37" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="E37" s="6" t="s">
-        <v>254</v>
-      </c>
-      <c r="F37" s="6" t="s">
+      <c r="E37" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="F37" s="11" t="s">
         <v>63</v>
       </c>
       <c r="G37" t="s">
@@ -6921,24 +6952,24 @@
         <v>63</v>
       </c>
       <c r="K37" t="s">
-        <v>255</v>
-      </c>
-      <c r="L37" s="7" t="s">
+        <v>256</v>
+      </c>
+      <c r="L37" t="s">
         <v>63</v>
       </c>
       <c r="M37" t="s">
         <v>63</v>
       </c>
       <c r="N37" s="12" t="s">
-        <v>256</v>
-      </c>
-      <c r="O37" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="P37" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q37" s="10" t="s">
+        <v>257</v>
+      </c>
+      <c r="O37" t="s">
+        <v>63</v>
+      </c>
+      <c r="P37" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q37" s="13" t="s">
         <v>133</v>
       </c>
       <c r="R37" t="s">
@@ -6947,26 +6978,26 @@
       <c r="S37" t="s">
         <v>167</v>
       </c>
-      <c r="T37" s="18" t="s">
-        <v>257</v>
+      <c r="T37" s="11" t="s">
+        <v>258</v>
       </c>
       <c r="U37" t="s">
         <v>63</v>
       </c>
-      <c r="V37" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W37" s="16" t="s">
+      <c r="V37" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="X37" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y37" s="16" t="s">
+      <c r="W37" s="13" t="s">
         <v>223</v>
       </c>
-      <c r="Z37" s="16" t="s">
-        <v>258</v>
+      <c r="X37" s="13" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y37" s="13" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z37" s="13" t="s">
+        <v>259</v>
       </c>
       <c r="AA37" t="s">
         <v>63</v>
@@ -6983,7 +7014,7 @@
     </row>
     <row r="38" spans="1:30">
       <c r="A38" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B38" s="3" t="s">
         <v>19</v>
@@ -6995,7 +7026,7 @@
         <v>21</v>
       </c>
       <c r="E38" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="F38" t="s">
         <v>63</v>
@@ -7013,25 +7044,25 @@
         <v>63</v>
       </c>
       <c r="K38" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="L38" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M38" t="s">
-        <v>262</v>
-      </c>
-      <c r="N38" s="13" t="s">
-        <v>256</v>
+        <v>263</v>
+      </c>
+      <c r="N38" s="16" t="s">
+        <v>257</v>
       </c>
       <c r="O38" t="s">
         <v>131</v>
       </c>
-      <c r="P38" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q38" s="15" t="s">
-        <v>243</v>
+      <c r="P38" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q38" s="18" t="s">
+        <v>244</v>
       </c>
       <c r="R38" t="s">
         <v>134</v>
@@ -7040,25 +7071,25 @@
         <v>167</v>
       </c>
       <c r="T38" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="U38" t="s">
         <v>63</v>
       </c>
-      <c r="V38" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W38" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="X38" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="Y38" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="Z38" s="16" t="s">
-        <v>224</v>
+      <c r="V38" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="W38" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="X38" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y38" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z38" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="AA38" t="s">
         <v>63</v>
@@ -7075,7 +7106,7 @@
     </row>
     <row r="39" spans="1:30">
       <c r="A39" s="7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>19</v>
@@ -7087,7 +7118,7 @@
         <v>21</v>
       </c>
       <c r="E39" s="6" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="F39" s="6" t="s">
         <v>63</v>
@@ -7105,7 +7136,7 @@
         <v>63</v>
       </c>
       <c r="K39" s="6" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="L39" s="6" t="s">
         <v>63</v>
@@ -7113,8 +7144,8 @@
       <c r="M39" t="s">
         <v>63</v>
       </c>
-      <c r="N39" s="12" t="s">
-        <v>256</v>
+      <c r="N39" s="15" t="s">
+        <v>257</v>
       </c>
       <c r="O39" s="7" t="s">
         <v>63</v>
@@ -7122,8 +7153,8 @@
       <c r="P39" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q39" s="16" t="s">
-        <v>243</v>
+      <c r="Q39" s="19" t="s">
+        <v>244</v>
       </c>
       <c r="R39" t="s">
         <v>63</v>
@@ -7132,25 +7163,25 @@
         <v>167</v>
       </c>
       <c r="T39" s="6" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="U39" t="s">
         <v>63</v>
       </c>
-      <c r="V39" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W39" s="16" t="s">
+      <c r="V39" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="X39" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y39" s="10" t="s">
-        <v>240</v>
-      </c>
-      <c r="Z39" s="10" t="s">
-        <v>224</v>
+      <c r="W39" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="X39" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y39" s="13" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z39" s="13" t="s">
+        <v>225</v>
       </c>
       <c r="AA39" t="s">
         <v>63</v>
@@ -7167,7 +7198,7 @@
     </row>
     <row r="40" spans="1:30">
       <c r="A40" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>19</v>
@@ -7179,7 +7210,7 @@
         <v>21</v>
       </c>
       <c r="E40" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="F40" t="s">
         <v>63</v>
@@ -7197,7 +7228,7 @@
         <v>63</v>
       </c>
       <c r="K40" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="L40" t="s">
         <v>63</v>
@@ -7205,8 +7236,8 @@
       <c r="M40" t="s">
         <v>63</v>
       </c>
-      <c r="N40" s="13" t="s">
-        <v>256</v>
+      <c r="N40" s="16" t="s">
+        <v>257</v>
       </c>
       <c r="O40" t="s">
         <v>63</v>
@@ -7214,7 +7245,7 @@
       <c r="P40" t="s">
         <v>63</v>
       </c>
-      <c r="Q40" s="15" t="s">
+      <c r="Q40" s="18" t="s">
         <v>133</v>
       </c>
       <c r="R40" t="s">
@@ -7229,20 +7260,20 @@
       <c r="U40" t="s">
         <v>63</v>
       </c>
-      <c r="V40" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W40" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="X40" s="16" t="s">
+      <c r="V40" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="W40" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="Y40" s="16" t="s">
-        <v>223</v>
-      </c>
-      <c r="Z40" s="16" t="s">
+      <c r="X40" s="19" t="s">
+        <v>237</v>
+      </c>
+      <c r="Y40" s="19" t="s">
         <v>224</v>
+      </c>
+      <c r="Z40" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="AA40" t="s">
         <v>63</v>
@@ -7259,7 +7290,7 @@
     </row>
     <row r="41" spans="1:30">
       <c r="A41" s="7" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="B41" s="3" t="s">
         <v>19</v>
@@ -7271,7 +7302,7 @@
         <v>21</v>
       </c>
       <c r="E41" s="6" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F41" t="s">
         <v>63</v>
@@ -7289,7 +7320,7 @@
         <v>63</v>
       </c>
       <c r="K41" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="L41" s="6" t="s">
         <v>63</v>
@@ -7297,7 +7328,7 @@
       <c r="M41" t="s">
         <v>63</v>
       </c>
-      <c r="N41" s="12" t="s">
+      <c r="N41" s="15" t="s">
         <v>186</v>
       </c>
       <c r="O41" s="7" t="s">
@@ -7306,8 +7337,8 @@
       <c r="P41" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q41" s="16" t="s">
-        <v>274</v>
+      <c r="Q41" s="19" t="s">
+        <v>275</v>
       </c>
       <c r="R41" t="s">
         <v>63</v>
@@ -7316,25 +7347,25 @@
         <v>167</v>
       </c>
       <c r="T41" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="U41" t="s">
         <v>63</v>
       </c>
-      <c r="V41" s="10" t="s">
-        <v>276</v>
-      </c>
-      <c r="W41" s="10" t="s">
+      <c r="V41" s="13" t="s">
         <v>277</v>
       </c>
-      <c r="X41" s="10" t="s">
-        <v>246</v>
-      </c>
-      <c r="Y41" s="10" t="s">
-        <v>210</v>
-      </c>
-      <c r="Z41" s="10" t="s">
-        <v>223</v>
+      <c r="W41" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="X41" s="13" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y41" s="13" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z41" s="13" t="s">
+        <v>224</v>
       </c>
       <c r="AA41" t="s">
         <v>63</v>
@@ -7351,7 +7382,7 @@
     </row>
     <row r="42" spans="1:30">
       <c r="A42" s="7" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>19</v>
@@ -7363,7 +7394,7 @@
         <v>21</v>
       </c>
       <c r="E42" s="6" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="F42" t="s">
         <v>63</v>
@@ -7381,7 +7412,7 @@
         <v>63</v>
       </c>
       <c r="K42" s="6" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="L42" s="7" t="s">
         <v>63</v>
@@ -7389,8 +7420,8 @@
       <c r="M42" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N42" s="12" t="s">
-        <v>281</v>
+      <c r="N42" s="15" t="s">
+        <v>282</v>
       </c>
       <c r="O42" s="7" t="s">
         <v>63</v>
@@ -7398,8 +7429,8 @@
       <c r="P42" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q42" s="16" t="s">
-        <v>199</v>
+      <c r="Q42" s="19" t="s">
+        <v>200</v>
       </c>
       <c r="R42" s="7" t="s">
         <v>63</v>
@@ -7408,25 +7439,25 @@
         <v>167</v>
       </c>
       <c r="T42" s="6" t="s">
-        <v>282</v>
-      </c>
-      <c r="U42" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="V42" s="16" t="s">
-        <v>244</v>
-      </c>
-      <c r="W42" s="16" t="s">
+        <v>283</v>
+      </c>
+      <c r="U42" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="V42" s="19" t="s">
         <v>245</v>
       </c>
-      <c r="X42" s="16" t="s">
+      <c r="W42" s="19" t="s">
         <v>246</v>
       </c>
-      <c r="Y42" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Z42" s="16" t="s">
-        <v>240</v>
+      <c r="X42" s="19" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y42" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="Z42" s="19" t="s">
+        <v>241</v>
       </c>
       <c r="AA42" t="s">
         <v>63</v>
@@ -7443,7 +7474,7 @@
     </row>
     <row r="43" spans="1:30">
       <c r="A43" s="7" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>19</v>
@@ -7455,7 +7486,7 @@
         <v>21</v>
       </c>
       <c r="E43" s="6" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="F43" t="s">
         <v>63</v>
@@ -7473,7 +7504,7 @@
         <v>63</v>
       </c>
       <c r="K43" s="6" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="L43" s="7" t="s">
         <v>63</v>
@@ -7481,7 +7512,7 @@
       <c r="M43" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N43" s="12" t="s">
+      <c r="N43" s="15" t="s">
         <v>186</v>
       </c>
       <c r="O43" s="7" t="s">
@@ -7490,8 +7521,8 @@
       <c r="P43" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q43" s="16" t="s">
-        <v>286</v>
+      <c r="Q43" s="19" t="s">
+        <v>287</v>
       </c>
       <c r="R43" s="7" t="s">
         <v>63</v>
@@ -7500,25 +7531,25 @@
         <v>167</v>
       </c>
       <c r="T43" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="U43" s="10" t="s">
-        <v>63</v>
-      </c>
-      <c r="V43" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W43" s="16" t="s">
+        <v>288</v>
+      </c>
+      <c r="U43" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="V43" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="X43" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y43" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z43" s="16" t="s">
+      <c r="W43" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="X43" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y43" s="19" t="s">
         <v>229</v>
+      </c>
+      <c r="Z43" s="19" t="s">
+        <v>230</v>
       </c>
       <c r="AA43" t="s">
         <v>63</v>
@@ -7535,7 +7566,7 @@
     </row>
     <row r="44" spans="1:30">
       <c r="A44" s="7" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B44" s="3" t="s">
         <v>19</v>
@@ -7547,7 +7578,7 @@
         <v>21</v>
       </c>
       <c r="E44" s="6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="F44" s="6" t="s">
         <v>63</v>
@@ -7565,7 +7596,7 @@
         <v>63</v>
       </c>
       <c r="K44" s="6" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="L44" s="7" t="s">
         <v>63</v>
@@ -7573,7 +7604,7 @@
       <c r="M44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="N44" s="12" t="s">
+      <c r="N44" s="15" t="s">
         <v>176</v>
       </c>
       <c r="O44" s="7" t="s">
@@ -7582,7 +7613,7 @@
       <c r="P44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="Q44" s="16" t="s">
+      <c r="Q44" s="19" t="s">
         <v>133</v>
       </c>
       <c r="R44" s="7" t="s">
@@ -7591,26 +7622,26 @@
       <c r="S44" s="7" t="s">
         <v>167</v>
       </c>
-      <c r="T44" s="18" t="s">
-        <v>257</v>
+      <c r="T44" s="21" t="s">
+        <v>291</v>
       </c>
       <c r="U44" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="V44" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W44" s="16" t="s">
-        <v>235</v>
-      </c>
-      <c r="X44" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="Y44" s="16" t="s">
-        <v>240</v>
-      </c>
-      <c r="Z44" s="16" t="s">
-        <v>224</v>
+      <c r="V44" s="13" t="s">
+        <v>222</v>
+      </c>
+      <c r="W44" s="19" t="s">
+        <v>236</v>
+      </c>
+      <c r="X44" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y44" s="19" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z44" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="AA44" t="s">
         <v>63</v>
@@ -7627,7 +7658,7 @@
     </row>
     <row r="45" spans="1:30">
       <c r="A45" t="s">
-        <v>290</v>
+        <v>292</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>19</v>
@@ -7639,7 +7670,7 @@
         <v>21</v>
       </c>
       <c r="E45" t="s">
-        <v>291</v>
+        <v>293</v>
       </c>
       <c r="F45" t="s">
         <v>63</v>
@@ -7657,25 +7688,25 @@
         <v>63</v>
       </c>
       <c r="K45" t="s">
-        <v>292</v>
+        <v>294</v>
       </c>
       <c r="L45" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>293</v>
-      </c>
-      <c r="N45" s="13" t="s">
+        <v>295</v>
+      </c>
+      <c r="N45" s="16" t="s">
         <v>186</v>
       </c>
       <c r="O45" t="s">
         <v>131</v>
       </c>
-      <c r="P45" s="13" t="s">
-        <v>263</v>
-      </c>
-      <c r="Q45" s="15" t="s">
-        <v>294</v>
+      <c r="P45" s="16" t="s">
+        <v>264</v>
+      </c>
+      <c r="Q45" s="18" t="s">
+        <v>296</v>
       </c>
       <c r="R45" t="s">
         <v>134</v>
@@ -7684,25 +7715,25 @@
         <v>167</v>
       </c>
       <c r="T45" s="4" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="U45" t="s">
         <v>63</v>
       </c>
-      <c r="V45" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W45" s="16" t="s">
+      <c r="V45" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="X45" s="16" t="s">
-        <v>210</v>
-      </c>
-      <c r="Y45" s="16" t="s">
+      <c r="W45" s="19" t="s">
         <v>223</v>
       </c>
-      <c r="Z45" s="16" t="s">
+      <c r="X45" s="19" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y45" s="19" t="s">
         <v>224</v>
+      </c>
+      <c r="Z45" s="19" t="s">
+        <v>225</v>
       </c>
       <c r="AA45" t="s">
         <v>63</v>
@@ -7719,7 +7750,7 @@
     </row>
     <row r="46" spans="1:30">
       <c r="A46" t="s">
-        <v>295</v>
+        <v>297</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>19</v>
@@ -7731,7 +7762,7 @@
         <v>21</v>
       </c>
       <c r="E46" t="s">
-        <v>296</v>
+        <v>298</v>
       </c>
       <c r="F46" t="s">
         <v>63</v>
@@ -7749,25 +7780,25 @@
         <v>63</v>
       </c>
       <c r="K46" t="s">
-        <v>297</v>
+        <v>299</v>
       </c>
       <c r="L46" t="s">
-        <v>298</v>
+        <v>300</v>
       </c>
       <c r="M46" s="4" t="s">
-        <v>299</v>
-      </c>
-      <c r="N46" s="13" t="s">
+        <v>301</v>
+      </c>
+      <c r="N46" s="16" t="s">
         <v>186</v>
       </c>
       <c r="O46" t="s">
         <v>131</v>
       </c>
-      <c r="P46" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q46" s="15" t="s">
-        <v>300</v>
+      <c r="P46" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q46" s="18" t="s">
+        <v>302</v>
       </c>
       <c r="R46" t="s">
         <v>134</v>
@@ -7776,25 +7807,25 @@
         <v>167</v>
       </c>
       <c r="T46" s="4" t="s">
-        <v>299</v>
+        <v>301</v>
       </c>
       <c r="U46" t="s">
         <v>63</v>
       </c>
-      <c r="V46" s="10" t="s">
-        <v>221</v>
-      </c>
-      <c r="W46" s="16" t="s">
+      <c r="V46" s="13" t="s">
         <v>222</v>
       </c>
-      <c r="X46" s="16" t="s">
-        <v>222</v>
-      </c>
-      <c r="Y46" s="16" t="s">
-        <v>228</v>
-      </c>
-      <c r="Z46" s="16" t="s">
-        <v>229</v>
+      <c r="W46" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="X46" s="19" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y46" s="19" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z46" s="19" t="s">
+        <v>259</v>
       </c>
       <c r="AA46" t="s">
         <v>63</v>
@@ -7813,7 +7844,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D2" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C2" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="C2" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B3" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D3" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C3" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
@@ -7854,9 +7885,6 @@
     <hyperlink ref="B23" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D23" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C23" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="B24" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="D24" r:id="rId2" display="Sah@6057"/>
-    <hyperlink ref="C24" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="M10" r:id="rId8" display="rahul@gamil.com"/>
     <hyperlink ref="B8" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="C8" r:id="rId4" display="amandeep.kamboj@testingxperts.com"/>
@@ -7935,9 +7963,6 @@
     <hyperlink ref="D36" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C36" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="B36" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="B37" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
-    <hyperlink ref="C37" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
-    <hyperlink ref="D37" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="B39" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="C39" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
     <hyperlink ref="D39" r:id="rId2" display="Sah@6057"/>
@@ -7954,6 +7979,12 @@
     <hyperlink ref="B14" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
     <hyperlink ref="D14" r:id="rId2" display="Sah@6057"/>
     <hyperlink ref="C14" r:id="rId3" display="sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B24" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="D24" r:id="rId2" display="Sah@6057"/>
+    <hyperlink ref="C24" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="B37" r:id="rId1" display="https://webapps.brightoutcome.com/acs3-hu/app/home" tooltip="https://webapps.brightoutcome.com/acs3-hu/app/home"/>
+    <hyperlink ref="C37" r:id="rId3" display="sahil.kapoor@testingxperts.com" tooltip="mailto:sahil.kapoor@testingxperts.com"/>
+    <hyperlink ref="D37" r:id="rId2" display="Sah@6057"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>